<commit_message>
Connor: Added layout for second Experiment
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
   <si>
     <t>First Request</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>System Proxy - BBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I will retry this with a slower internet connection as it would follow if you have a fast connection that there would not be much of a difference between </t>
   </si>
 </sst>
 </file>
@@ -85,13 +88,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,7 +533,263 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1520754464"/>
+        <c:axId val="1617533696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1520754464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1617533696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1617533696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1520754464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1073,20 +1332,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1106,6 +1868,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28F363CC-A40D-4B4B-B7EA-E84F65872B97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1411,10 +2211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,11 +2286,11 @@
         <v>7</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="3"/>
       <c r="H8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1775,12 +2575,191 @@
         <v>1.7139999999999997</v>
       </c>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="H31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" t="e">
+        <f>AVERAGE(B33:B42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C43" t="e">
+        <f t="shared" ref="C43:F43" si="2">AVERAGE(C33:C42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E43" t="e">
+        <f t="shared" ref="E43:H43" si="3">AVERAGE(E33:E42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F43" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H43" t="e">
+        <f>AVERAGE(H33:H42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I43" t="e">
+        <f t="shared" ref="I43" si="4">AVERAGE(I33:I42)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H31:I31"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="A1:F6"/>
     <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A23:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1860,11 +2839,11 @@
         <v>4</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">

</xml_diff>

<commit_message>
Connor: Updated Caching Experiment
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="WebViewMeasurement" sheetId="1" r:id="rId1"/>
@@ -554,6 +554,142 @@
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Electron Proxy First Request</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>WebViewMeasurement!$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>18.519000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-10E3-49B1-9BCD-DFE3F6CB517E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Electron Proxy Second Request</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>WebViewMeasurement!$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.0080000000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-10E3-49B1-9BCD-DFE3F6CB517E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>No Proxy First Request</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>WebViewMeasurement!$E$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>9.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-10E3-49B1-9BCD-DFE3F6CB517E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>No Proxy Second Request</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>WebViewMeasurement!$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10.37142857142857</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-10E3-49B1-9BCD-DFE3F6CB517E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2213,22 +2349,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2238,7 +2374,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2246,7 +2382,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2254,7 +2390,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2262,7 +2398,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2270,7 +2406,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2278,7 +2414,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2296,7 +2432,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -2316,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2339,7 +2475,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2362,7 +2498,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
@@ -2385,7 +2521,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4</v>
       </c>
@@ -2408,7 +2544,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5</v>
       </c>
@@ -2431,7 +2567,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>6</v>
       </c>
@@ -2454,7 +2590,7 @@
         <v>1.59</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>7</v>
       </c>
@@ -2477,7 +2613,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>8</v>
       </c>
@@ -2500,7 +2636,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>9</v>
       </c>
@@ -2523,7 +2659,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>10</v>
       </c>
@@ -2546,7 +2682,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2575,7 +2711,7 @@
         <v>1.7139999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2585,7 +2721,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2593,7 +2729,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2601,7 +2737,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2609,7 +2745,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2617,7 +2753,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2625,7 +2761,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2633,7 +2769,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -2651,7 +2787,7 @@
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -2671,75 +2807,177 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>16.59</v>
+      </c>
+      <c r="C33">
+        <v>4.25</v>
+      </c>
+      <c r="E33">
+        <v>11.56</v>
+      </c>
+      <c r="F33">
+        <v>11.35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>12.44</v>
+      </c>
+      <c r="C34">
+        <v>4.13</v>
+      </c>
+      <c r="E34">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="F34">
+        <v>8.9600000000000009</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>23.88</v>
+      </c>
+      <c r="C35">
+        <v>3.98</v>
+      </c>
+      <c r="E35">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="F35">
+        <v>13.27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>23.64</v>
+      </c>
+      <c r="C36">
+        <v>4.17</v>
+      </c>
+      <c r="E36">
+        <v>9.43</v>
+      </c>
+      <c r="F36">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>19.12</v>
+      </c>
+      <c r="C37">
+        <v>4.18</v>
+      </c>
+      <c r="E37">
+        <v>10.02</v>
+      </c>
+      <c r="F37">
+        <v>11.38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>20.45</v>
+      </c>
+      <c r="C38">
+        <v>6.94</v>
+      </c>
+      <c r="E38">
+        <v>9.5</v>
+      </c>
+      <c r="F38">
+        <v>9.64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>16.21</v>
+      </c>
+      <c r="C39">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="E39">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="F39">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>20.46</v>
+      </c>
+      <c r="C40">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>16.41</v>
+      </c>
+      <c r="C41">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>15.99</v>
+      </c>
+      <c r="C42">
+        <v>7.06</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>3</v>
       </c>
-      <c r="B43" t="e">
+      <c r="B43">
         <f>AVERAGE(B33:B42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C43" t="e">
-        <f t="shared" ref="C43:F43" si="2">AVERAGE(C33:C42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E43" t="e">
-        <f t="shared" ref="E43:H43" si="3">AVERAGE(E33:E42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F43" t="e">
+        <v>18.519000000000002</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ref="C43" si="2">AVERAGE(C33:C42)</f>
+        <v>5.0080000000000009</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ref="E43:F43" si="3">AVERAGE(E33:E42)</f>
+        <v>9.85</v>
+      </c>
+      <c r="F43">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>10.37142857142857</v>
       </c>
       <c r="H43" t="e">
         <f>AVERAGE(H33:H42)</f>
@@ -2752,14 +2990,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:F6"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A23:F29"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A1:F6"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A23:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2774,16 +3012,16 @@
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2791,7 +3029,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2799,7 +3037,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2807,7 +3045,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2815,7 +3053,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2823,7 +3061,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2831,7 +3069,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2845,7 +3083,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -2859,57 +3097,57 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Connor: Added clear cache button to Caching application to allow for tests to be run
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="WebViewMeasurement" sheetId="1" r:id="rId1"/>
     <sheet name="ApacheBenchmark" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,9 +41,6 @@
     <t>No Proxy - BBC</t>
   </si>
   <si>
-    <t>To do this experiment I set the expiry time for the cache to be 30 seconds. After each 30 seconds I made a request and measured the first response time and then made a second request measuring that response time also. I left the applications running throughout (Client and Edge). This measurement was taken my recording the start time and end time of the request from the WebView element event handlers</t>
-  </si>
-  <si>
     <t>Electron Proxy - BBC</t>
   </si>
   <si>
@@ -50,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">I will retry this with a slower internet connection as it would follow if you have a fast connection that there would not be much of a difference between </t>
+  </si>
+  <si>
+    <t>To do this experiment I set the expiry time for the cache to be 30 seconds. After each 30 seconds I made a request and measured the first response time and then made a second request measuring that response time also. I left the applications running throughout (Client and Edge). This measurement was taken my recording the start time and end time of the request from the WebView element event handlers. Running on the Client Pi</t>
   </si>
 </sst>
 </file>
@@ -157,7 +158,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8.7689999999999984</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -191,7 +192,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.2640000000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -225,7 +226,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.081</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -259,7 +260,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.6600000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -293,7 +294,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.8220000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -327,7 +328,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.7139999999999997</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2349,24 +2350,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2374,7 +2375,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2382,7 +2383,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2390,7 +2391,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2398,7 +2399,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2406,7 +2407,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2414,12 +2415,12 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
@@ -2428,11 +2429,11 @@
       </c>
       <c r="F8" s="3"/>
       <c r="H8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -2452,268 +2453,88 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10">
-        <v>4.62</v>
-      </c>
-      <c r="C10">
-        <v>3.78</v>
-      </c>
-      <c r="E10">
-        <v>2.44</v>
-      </c>
-      <c r="F10">
-        <v>1.63</v>
-      </c>
-      <c r="H10">
-        <v>2.75</v>
-      </c>
-      <c r="I10">
-        <v>2.0299999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11">
-        <v>23.43</v>
-      </c>
-      <c r="C11">
-        <v>8.36</v>
-      </c>
-      <c r="E11">
-        <v>1.74</v>
-      </c>
-      <c r="F11">
-        <v>1.47</v>
-      </c>
-      <c r="H11">
-        <v>3.57</v>
-      </c>
-      <c r="I11">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12">
-        <v>3.99</v>
-      </c>
-      <c r="C12">
-        <v>1.36</v>
-      </c>
-      <c r="E12">
-        <v>3.36</v>
-      </c>
-      <c r="F12">
-        <v>2.29</v>
-      </c>
-      <c r="H12">
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="I12">
-        <v>1.66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
-      <c r="B13">
-        <v>19.86</v>
-      </c>
-      <c r="C13">
-        <v>17.440000000000001</v>
-      </c>
-      <c r="E13">
-        <v>2.96</v>
-      </c>
-      <c r="F13">
-        <v>2.08</v>
-      </c>
-      <c r="H13">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="I13">
-        <v>1.56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
-      <c r="B14">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="C14">
-        <v>1.61</v>
-      </c>
-      <c r="E14">
-        <v>1.7</v>
-      </c>
-      <c r="F14">
-        <v>1.76</v>
-      </c>
-      <c r="H14">
-        <v>2.62</v>
-      </c>
-      <c r="I14">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
-      <c r="B15">
-        <v>5.96</v>
-      </c>
-      <c r="C15">
-        <v>2.7</v>
-      </c>
-      <c r="E15">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="F15">
-        <v>1.49</v>
-      </c>
-      <c r="H15">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="I15">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
-      <c r="B16">
-        <v>6.95</v>
-      </c>
-      <c r="C16">
-        <v>1.84</v>
-      </c>
-      <c r="E16">
-        <v>1.57</v>
-      </c>
-      <c r="F16">
-        <v>1.48</v>
-      </c>
-      <c r="H16">
-        <v>2.72</v>
-      </c>
-      <c r="I16">
-        <v>1.79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
-      <c r="B17">
-        <v>4.38</v>
-      </c>
-      <c r="C17">
-        <v>1.55</v>
-      </c>
-      <c r="E17">
-        <v>1.35</v>
-      </c>
-      <c r="F17">
-        <v>1.42</v>
-      </c>
-      <c r="H17">
-        <v>2.79</v>
-      </c>
-      <c r="I17">
-        <v>2.33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
-      <c r="B18">
-        <v>4.41</v>
-      </c>
-      <c r="C18">
-        <v>2.04</v>
-      </c>
-      <c r="E18">
-        <v>2.06</v>
-      </c>
-      <c r="F18">
-        <v>1.56</v>
-      </c>
-      <c r="H18">
-        <v>2.7</v>
-      </c>
-      <c r="I18">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
-      <c r="B19">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="C19">
-        <v>1.96</v>
-      </c>
-      <c r="E19">
-        <v>1.56</v>
-      </c>
-      <c r="F19">
-        <v>1.42</v>
-      </c>
-      <c r="H19">
-        <v>2.25</v>
-      </c>
-      <c r="I19">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="e">
         <f>AVERAGE(B10:B19)</f>
-        <v>8.7689999999999984</v>
-      </c>
-      <c r="C20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C20" t="e">
         <f t="shared" ref="C20:F20" si="0">AVERAGE(C10:C19)</f>
-        <v>4.2640000000000002</v>
-      </c>
-      <c r="E20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E20" t="e">
         <f t="shared" si="0"/>
-        <v>2.081</v>
-      </c>
-      <c r="F20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" t="e">
         <f t="shared" si="0"/>
-        <v>1.6600000000000001</v>
-      </c>
-      <c r="H20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" t="e">
         <f>AVERAGE(H10:H19)</f>
-        <v>2.8220000000000001</v>
-      </c>
-      <c r="I20">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" t="e">
         <f t="shared" ref="I20" si="1">AVERAGE(I10:I19)</f>
-        <v>1.7139999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2721,7 +2542,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2729,7 +2550,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2737,7 +2558,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2745,7 +2566,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2753,7 +2574,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2761,7 +2582,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2769,12 +2590,12 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="1"/>
@@ -2783,11 +2604,11 @@
       </c>
       <c r="F31" s="3"/>
       <c r="H31" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -2807,7 +2628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2824,7 +2645,7 @@
         <v>11.35</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2841,7 +2662,7 @@
         <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2858,7 +2679,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2875,7 +2696,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5</v>
       </c>
@@ -2892,7 +2713,7 @@
         <v>11.38</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6</v>
       </c>
@@ -2909,7 +2730,7 @@
         <v>9.64</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7</v>
       </c>
@@ -2926,7 +2747,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2937,7 +2758,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9</v>
       </c>
@@ -2948,7 +2769,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>10</v>
       </c>
@@ -2959,7 +2780,7 @@
         <v>7.06</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -3012,16 +2833,16 @@
       <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3029,7 +2850,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3037,7 +2858,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3045,7 +2866,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -3053,7 +2874,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -3061,7 +2882,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3069,7 +2890,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -3083,7 +2904,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -3097,57 +2918,57 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Connor: Updated caching application to allow for easier experimentation, also included updated experiment results. I added the file where I shall write my Dissertation and added the title page. I updated the Machine Learning application so that it can save and process the most common string sent. This request is intercepted by the Edge Node so it will need to be updated to do some pre processing
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="WebViewMeasurement" sheetId="1" r:id="rId1"/>
     <sheet name="ApacheBenchmark" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>First Request</t>
   </si>
@@ -45,12 +44,6 @@
   </si>
   <si>
     <t>System Proxy - BBC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I will retry this with a slower internet connection as it would follow if you have a fast connection that there would not be much of a difference between </t>
-  </si>
-  <si>
-    <t>To do this experiment I set the expiry time for the cache to be 30 seconds. After each 30 seconds I made a request and measured the first response time and then made a second request measuring that response time also. I left the applications running throughout (Client and Edge). This measurement was taken my recording the start time and end time of the request from the WebView element event handlers. Running on the Client Pi</t>
   </si>
 </sst>
 </file>
@@ -158,7 +151,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -192,7 +185,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5.003000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -226,7 +219,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.6166666666666654</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -260,7 +253,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.8233333333333324</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,7 +571,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>18.519000000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -612,7 +605,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.0080000000000009</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -646,7 +639,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.85</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -680,7 +673,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10.37142857142857</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2351,7 +2344,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2366,9 +2359,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -2457,71 +2448,149 @@
       <c r="A10">
         <v>1</v>
       </c>
+      <c r="B10">
+        <v>8.4</v>
+      </c>
+      <c r="C10">
+        <v>5.28</v>
+      </c>
+      <c r="E10">
+        <v>8.85</v>
+      </c>
+      <c r="F10">
+        <v>8.86</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
+      <c r="B11">
+        <v>4.58</v>
+      </c>
+      <c r="C11">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E11">
+        <v>8.41</v>
+      </c>
+      <c r="F11">
+        <v>8.52</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
+      <c r="B12">
+        <v>5.35</v>
+      </c>
+      <c r="C12">
+        <v>4.96</v>
+      </c>
+      <c r="E12">
+        <v>8.59</v>
+      </c>
+      <c r="F12">
+        <v>9.09</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
+      <c r="B13">
+        <v>5.35</v>
+      </c>
+      <c r="C13">
+        <v>5.23</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
+      <c r="B14">
+        <v>5.34</v>
+      </c>
+      <c r="C14">
+        <v>5.21</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
+      <c r="B15">
+        <v>8.25</v>
+      </c>
+      <c r="C15">
+        <v>4.16</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
+      <c r="B16">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="C16">
+        <v>5.09</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
+      <c r="B17">
+        <v>9.61</v>
+      </c>
+      <c r="C17">
+        <v>4.67</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
+      <c r="B18">
+        <v>5.22</v>
+      </c>
+      <c r="C18">
+        <v>5.07</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
+      <c r="B19">
+        <v>6.62</v>
+      </c>
+      <c r="C19">
+        <v>5.38</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="B20" t="e">
+      <c r="B20">
         <f>AVERAGE(B10:B19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C20" t="e">
+        <v>6.7</v>
+      </c>
+      <c r="C20">
         <f t="shared" ref="C20:F20" si="0">AVERAGE(C10:C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" t="e">
+        <v>5.003000000000001</v>
+      </c>
+      <c r="E20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F20" t="e">
+        <v>8.6166666666666654</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>8.8233333333333324</v>
       </c>
       <c r="H20" t="e">
         <f>AVERAGE(H10:H19)</f>
@@ -2533,9 +2602,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2632,173 +2699,71 @@
       <c r="A33">
         <v>1</v>
       </c>
-      <c r="B33">
-        <v>16.59</v>
-      </c>
-      <c r="C33">
-        <v>4.25</v>
-      </c>
-      <c r="E33">
-        <v>11.56</v>
-      </c>
-      <c r="F33">
-        <v>11.35</v>
-      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
-      <c r="B34">
-        <v>12.44</v>
-      </c>
-      <c r="C34">
-        <v>4.13</v>
-      </c>
-      <c r="E34">
-        <v>9.7899999999999991</v>
-      </c>
-      <c r="F34">
-        <v>8.9600000000000009</v>
-      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
-      <c r="B35">
-        <v>23.88</v>
-      </c>
-      <c r="C35">
-        <v>3.98</v>
-      </c>
-      <c r="E35">
-        <v>9.6199999999999992</v>
-      </c>
-      <c r="F35">
-        <v>13.27</v>
-      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
-      <c r="B36">
-        <v>23.64</v>
-      </c>
-      <c r="C36">
-        <v>4.17</v>
-      </c>
-      <c r="E36">
-        <v>9.43</v>
-      </c>
-      <c r="F36">
-        <v>9.3000000000000007</v>
-      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5</v>
       </c>
-      <c r="B37">
-        <v>19.12</v>
-      </c>
-      <c r="C37">
-        <v>4.18</v>
-      </c>
-      <c r="E37">
-        <v>10.02</v>
-      </c>
-      <c r="F37">
-        <v>11.38</v>
-      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6</v>
       </c>
-      <c r="B38">
-        <v>20.45</v>
-      </c>
-      <c r="C38">
-        <v>6.94</v>
-      </c>
-      <c r="E38">
-        <v>9.5</v>
-      </c>
-      <c r="F38">
-        <v>9.64</v>
-      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7</v>
       </c>
-      <c r="B39">
-        <v>16.21</v>
-      </c>
-      <c r="C39">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="E39">
-        <v>9.0299999999999994</v>
-      </c>
-      <c r="F39">
-        <v>8.6999999999999993</v>
-      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>8</v>
       </c>
-      <c r="B40">
-        <v>20.46</v>
-      </c>
-      <c r="C40">
-        <v>4.08</v>
-      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9</v>
       </c>
-      <c r="B41">
-        <v>16.41</v>
-      </c>
-      <c r="C41">
-        <v>7.1</v>
-      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>10</v>
       </c>
-      <c r="B42">
-        <v>15.99</v>
-      </c>
-      <c r="C42">
-        <v>7.06</v>
-      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
-      <c r="B43">
+      <c r="B43" t="e">
         <f>AVERAGE(B33:B42)</f>
-        <v>18.519000000000002</v>
-      </c>
-      <c r="C43">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C43" t="e">
         <f t="shared" ref="C43" si="2">AVERAGE(C33:C42)</f>
-        <v>5.0080000000000009</v>
-      </c>
-      <c r="E43">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E43" t="e">
         <f t="shared" ref="E43:F43" si="3">AVERAGE(E33:E42)</f>
-        <v>9.85</v>
-      </c>
-      <c r="F43">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F43" t="e">
         <f t="shared" si="3"/>
-        <v>10.37142857142857</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H43" t="e">
         <f>AVERAGE(H33:H42)</f>

</xml_diff>

<commit_message>
Connor: Updated KMeans evaluation to return the first section of each cluster. Also updated the Dissertation.docx and removed previous test results from the caching application.
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12645"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="8">
   <si>
     <t>First Request</t>
   </si>
@@ -150,9 +150,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>6.7</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -184,9 +181,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5.003000000000001</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -219,7 +213,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8.6166666666666654</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -253,7 +247,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8.8233333333333324</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2341,10 +2335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R57" sqref="R57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2448,149 +2442,63 @@
       <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10">
-        <v>8.4</v>
-      </c>
-      <c r="C10">
-        <v>5.28</v>
-      </c>
-      <c r="E10">
-        <v>8.85</v>
-      </c>
-      <c r="F10">
-        <v>8.86</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11">
-        <v>4.58</v>
-      </c>
-      <c r="C11">
-        <v>4.9800000000000004</v>
-      </c>
-      <c r="E11">
-        <v>8.41</v>
-      </c>
-      <c r="F11">
-        <v>8.52</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12">
-        <v>5.35</v>
-      </c>
-      <c r="C12">
-        <v>4.96</v>
-      </c>
-      <c r="E12">
-        <v>8.59</v>
-      </c>
-      <c r="F12">
-        <v>9.09</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
-      <c r="B13">
-        <v>5.35</v>
-      </c>
-      <c r="C13">
-        <v>5.23</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
-      <c r="B14">
-        <v>5.34</v>
-      </c>
-      <c r="C14">
-        <v>5.21</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
-      <c r="B15">
-        <v>8.25</v>
-      </c>
-      <c r="C15">
-        <v>4.16</v>
-      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
-      <c r="B16">
-        <v>8.2799999999999994</v>
-      </c>
-      <c r="C16">
-        <v>5.09</v>
-      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
-      <c r="B17">
-        <v>9.61</v>
-      </c>
-      <c r="C17">
-        <v>4.67</v>
-      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
-      <c r="B18">
-        <v>5.22</v>
-      </c>
-      <c r="C18">
-        <v>5.07</v>
-      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
-      <c r="B19">
-        <v>6.62</v>
-      </c>
-      <c r="C19">
-        <v>5.38</v>
-      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="B20">
-        <f>AVERAGE(B10:B19)</f>
-        <v>6.7</v>
-      </c>
-      <c r="C20">
-        <f t="shared" ref="C20:F20" si="0">AVERAGE(C10:C19)</f>
-        <v>5.003000000000001</v>
-      </c>
-      <c r="E20">
+      <c r="E20" t="e">
+        <f t="shared" ref="C20:F20" si="0">AVERAGE(E10:E19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" t="e">
         <f t="shared" si="0"/>
-        <v>8.6166666666666654</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>8.8233333333333324</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H20" t="e">
         <f>AVERAGE(H10:H19)</f>
@@ -2774,8 +2682,185 @@
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" s="3"/>
+      <c r="H54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" t="e">
+        <f>AVERAGE(B56:B65)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C66" t="e">
+        <f t="shared" ref="C66" si="5">AVERAGE(C56:C65)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E66" t="e">
+        <f t="shared" ref="E66:F66" si="6">AVERAGE(E56:E65)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F66" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H66" t="e">
+        <f>AVERAGE(H56:H65)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I66" t="e">
+        <f t="shared" ref="I66" si="7">AVERAGE(I56:I65)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="A46:F52"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="H54:I54"/>
     <mergeCell ref="A1:F6"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="A23:F29"/>

</xml_diff>

<commit_message>
Connor: Updated write up on experiments in Dissertation.docx.
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="33">
   <si>
     <t>First Request</t>
   </si>
@@ -108,6 +108,18 @@
   <si>
     <t>% Diff First/Second</t>
   </si>
+  <si>
+    <t>Average FirstSecond</t>
+  </si>
+  <si>
+    <t>Average Cache/NoCache</t>
+  </si>
+  <si>
+    <t>% Diff on no cache</t>
+  </si>
+  <si>
+    <t>% Diff on cached</t>
+  </si>
 </sst>
 </file>
 
@@ -150,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -166,12 +178,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2510,7 +2528,7 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>304801</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>67918</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2881,15 +2899,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J153"/>
+  <dimension ref="A1:J156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -2948,19 +2966,19 @@
         <v>22</v>
       </c>
       <c r="B3" s="5">
-        <f>AVERAGE(B21,B37,B53,B69,B85)</f>
+        <f>AVERAGE(B24,B40,B56,B72,B88)</f>
         <v>3.6980000000000004</v>
       </c>
       <c r="C3" s="2">
-        <f>AVERAGE(C21,C37,C53,C69,C85)</f>
+        <f>AVERAGE(C24,C40,C56,C72,C88)</f>
         <v>6.0133999999999999</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:J3" si="0">AVERAGE(D21,D37,D53,D69,D85)</f>
+        <f t="shared" ref="D3:J3" si="0">AVERAGE(D24,D40,D56,D72,D88)</f>
         <v>4.6429999999999998</v>
       </c>
       <c r="E3" s="5">
-        <f>AVERAGE(E21,E37,E53,E69,E85)</f>
+        <f>AVERAGE(E24,E40,E56,E72,E88)</f>
         <v>3.7350000000000003</v>
       </c>
       <c r="F3" s="3">
@@ -2989,15 +3007,15 @@
         <v>12</v>
       </c>
       <c r="B4" s="5">
-        <f>AVERAGE(B22,B38,B54,B70,B86)</f>
+        <f>AVERAGE(B25,B41,B57,B73,B89)</f>
         <v>0.3434581313993238</v>
       </c>
       <c r="C4" s="2">
-        <f>AVERAGE(C22,C38,C54,C70,C86)</f>
+        <f>AVERAGE(C25,C41,C57,C73,C89)</f>
         <v>2.0317741364660522</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:J4" si="1">AVERAGE(D22,D38,D54,D70,D86)</f>
+        <f t="shared" ref="D4:J4" si="1">AVERAGE(D25,D41,D57,D73,D89)</f>
         <v>0.17686272071649228</v>
       </c>
       <c r="E4" s="5">
@@ -3029,275 +3047,238 @@
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <f>(C3-D3)/D3</f>
         <v>0.29515399526168429</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7">
         <f>(F3-G3)/G3</f>
         <v>0.34481292517006773</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7">
         <f>(I3-J3)/J3</f>
         <v>0.17856401743100242</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="8">
+        <v>31</v>
+      </c>
+      <c r="B6" s="7">
         <f>(B3-D3)/D3</f>
         <v>-0.20353219900926114</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7">
         <f>(E3-G3)/G3</f>
         <v>-7.4936224489794753E-3</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7">
         <f>(H3-J3)/J3</f>
         <v>-0.16663208134467727</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="7">
+        <f>(D3-B3)/B3</f>
+        <v>0.25554353704705229</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7">
+        <f t="shared" ref="E7" si="2">(G3-E3)/E3</f>
+        <v>7.5502008032127324E-3</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7">
+        <f t="shared" ref="H7" si="3">(J3-H3)/H3</f>
+        <v>0.19995019920318721</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="10">
+        <f>AVERAGE(B5:J5)</f>
+        <v>0.27284364595425142</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="10">
+        <f>AVERAGE(B6:J6)</f>
+        <v>-0.12588596760097262</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="10">
+        <f>AVERAGE(B7:J7)</f>
+        <v>0.15434797901781741</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="7" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="I9" s="6" t="s">
+      <c r="G12" s="9"/>
+      <c r="I12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>0</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D13" t="s">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E13" t="s">
         <v>23</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F13" t="s">
         <v>0</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G13" t="s">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H13" t="s">
         <v>23</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I13" t="s">
         <v>0</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J13" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>3.46</v>
-      </c>
-      <c r="C11">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D11">
-        <v>4.71</v>
-      </c>
-      <c r="E11">
-        <v>3.77</v>
-      </c>
-      <c r="F11">
-        <v>4.79</v>
-      </c>
-      <c r="G11">
-        <v>3.46</v>
-      </c>
-      <c r="H11">
-        <v>1.59</v>
-      </c>
-      <c r="I11">
-        <v>2.65</v>
-      </c>
-      <c r="J11">
-        <v>1.84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>3.93</v>
-      </c>
-      <c r="C12">
-        <v>8.49</v>
-      </c>
-      <c r="D12">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="E12">
-        <v>3.72</v>
-      </c>
-      <c r="F12">
-        <v>6.21</v>
-      </c>
-      <c r="G12">
-        <v>3.55</v>
-      </c>
-      <c r="H12">
-        <v>1.58</v>
-      </c>
-      <c r="I12">
-        <v>2.34</v>
-      </c>
-      <c r="J12">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>3.62</v>
-      </c>
-      <c r="C13">
-        <v>8.24</v>
-      </c>
-      <c r="D13">
-        <v>4.5</v>
-      </c>
-      <c r="E13">
-        <v>3.93</v>
-      </c>
-      <c r="F13">
-        <v>3.93</v>
-      </c>
-      <c r="G13">
-        <v>3.64</v>
-      </c>
-      <c r="H13">
-        <v>1.62</v>
-      </c>
-      <c r="I13">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="J13">
-        <v>1.86</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B14">
-        <v>3.34</v>
+        <v>3.46</v>
       </c>
       <c r="C14">
-        <v>4.93</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D14">
-        <v>4.6399999999999997</v>
+        <v>4.71</v>
       </c>
       <c r="E14">
-        <v>3.75</v>
+        <v>3.77</v>
       </c>
       <c r="F14">
-        <v>4.87</v>
+        <v>4.79</v>
       </c>
       <c r="G14">
-        <v>3.44</v>
+        <v>3.46</v>
       </c>
       <c r="H14">
-        <v>1.66</v>
+        <v>1.59</v>
       </c>
       <c r="I14">
-        <v>2.21</v>
+        <v>2.65</v>
       </c>
       <c r="J14">
-        <v>1.88</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>6.66</v>
+        <v>3.93</v>
       </c>
       <c r="C15">
-        <v>4.9000000000000004</v>
+        <v>8.49</v>
       </c>
       <c r="D15">
-        <v>4.9400000000000004</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="E15">
-        <v>3.56</v>
+        <v>3.72</v>
       </c>
       <c r="F15">
-        <v>9.73</v>
+        <v>6.21</v>
       </c>
       <c r="G15">
-        <v>3.45</v>
+        <v>3.55</v>
       </c>
       <c r="H15">
-        <v>1.61</v>
+        <v>1.58</v>
       </c>
       <c r="I15">
-        <v>2.19</v>
+        <v>2.34</v>
       </c>
       <c r="J15">
         <v>1.86</v>
@@ -3305,63 +3286,63 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>3.44</v>
+        <v>3.62</v>
       </c>
       <c r="C16">
-        <v>8.08</v>
+        <v>8.24</v>
       </c>
       <c r="D16">
-        <v>4.66</v>
+        <v>4.5</v>
       </c>
       <c r="E16">
-        <v>3.73</v>
+        <v>3.93</v>
       </c>
       <c r="F16">
         <v>3.93</v>
       </c>
       <c r="G16">
-        <v>4.05</v>
+        <v>3.64</v>
       </c>
       <c r="H16">
-        <v>1.68</v>
+        <v>1.62</v>
       </c>
       <c r="I16">
-        <v>2.21</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="J16">
-        <v>1.87</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B17">
-        <v>4.04</v>
+        <v>3.34</v>
       </c>
       <c r="C17">
-        <v>4.25</v>
+        <v>4.93</v>
       </c>
       <c r="D17">
-        <v>4.93</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="E17">
-        <v>3.57</v>
+        <v>3.75</v>
       </c>
       <c r="F17">
-        <v>4.34</v>
+        <v>4.87</v>
       </c>
       <c r="G17">
-        <v>3.5</v>
+        <v>3.44</v>
       </c>
       <c r="H17">
-        <v>1.58</v>
+        <v>1.66</v>
       </c>
       <c r="I17">
-        <v>2.59</v>
+        <v>2.21</v>
       </c>
       <c r="J17">
         <v>1.88</v>
@@ -3369,2168 +3350,2267 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B18">
-        <v>3.57</v>
+        <v>6.66</v>
       </c>
       <c r="C18">
-        <v>8.8800000000000008</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D18">
-        <v>4.95</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="E18">
-        <v>3.68</v>
+        <v>3.56</v>
       </c>
       <c r="F18">
-        <v>9.8000000000000007</v>
+        <v>9.73</v>
       </c>
       <c r="G18">
-        <v>3.9</v>
+        <v>3.45</v>
       </c>
       <c r="H18">
-        <v>1.62</v>
+        <v>1.61</v>
       </c>
       <c r="I18">
-        <v>2.25</v>
+        <v>2.19</v>
       </c>
       <c r="J18">
-        <v>1.87</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>3.53</v>
+        <v>3.44</v>
       </c>
       <c r="C19">
-        <v>8.32</v>
+        <v>8.08</v>
       </c>
       <c r="D19">
-        <v>4.8899999999999997</v>
+        <v>4.66</v>
       </c>
       <c r="E19">
-        <v>3.65</v>
+        <v>3.73</v>
       </c>
       <c r="F19">
-        <v>3.87</v>
+        <v>3.93</v>
       </c>
       <c r="G19">
-        <v>3.58</v>
+        <v>4.05</v>
       </c>
       <c r="H19">
-        <v>1.58</v>
+        <v>1.68</v>
       </c>
       <c r="I19">
-        <v>2.37</v>
+        <v>2.21</v>
       </c>
       <c r="J19">
-        <v>1.86</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>4.04</v>
+      </c>
+      <c r="C20">
+        <v>4.25</v>
+      </c>
+      <c r="D20">
+        <v>4.93</v>
+      </c>
+      <c r="E20">
+        <v>3.57</v>
+      </c>
+      <c r="F20">
+        <v>4.34</v>
+      </c>
+      <c r="G20">
+        <v>3.5</v>
+      </c>
+      <c r="H20">
+        <v>1.58</v>
+      </c>
+      <c r="I20">
+        <v>2.59</v>
+      </c>
+      <c r="J20">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>3.57</v>
+      </c>
+      <c r="C21">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="D21">
+        <v>4.95</v>
+      </c>
+      <c r="E21">
+        <v>3.68</v>
+      </c>
+      <c r="F21">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G21">
+        <v>3.9</v>
+      </c>
+      <c r="H21">
+        <v>1.62</v>
+      </c>
+      <c r="I21">
+        <v>2.25</v>
+      </c>
+      <c r="J21">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>3.53</v>
+      </c>
+      <c r="C22">
+        <v>8.32</v>
+      </c>
+      <c r="D22">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="E22">
+        <v>3.65</v>
+      </c>
+      <c r="F22">
+        <v>3.87</v>
+      </c>
+      <c r="G22">
+        <v>3.58</v>
+      </c>
+      <c r="H22">
+        <v>1.58</v>
+      </c>
+      <c r="I22">
+        <v>2.37</v>
+      </c>
+      <c r="J22">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>10</v>
       </c>
-      <c r="B20">
+      <c r="B23">
         <v>3.94</v>
       </c>
-      <c r="C20">
+      <c r="C23">
         <v>4.3499999999999996</v>
       </c>
-      <c r="D20">
+      <c r="D23">
         <v>4.54</v>
       </c>
-      <c r="E20">
+      <c r="E23">
         <v>3.54</v>
       </c>
-      <c r="F20">
+      <c r="F23">
         <v>4.6399999999999997</v>
       </c>
-      <c r="G20">
+      <c r="G23">
         <v>3.46</v>
       </c>
-      <c r="H20">
+      <c r="H23">
         <v>1.66</v>
       </c>
-      <c r="I20">
+      <c r="I23">
         <v>3.15</v>
       </c>
-      <c r="J20">
+      <c r="J23">
         <v>1.92</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>3</v>
       </c>
-      <c r="B21">
-        <f t="shared" ref="B21:D21" si="2">AVERAGE(B11:B20)</f>
+      <c r="B24">
+        <f t="shared" ref="B24:D24" si="4">AVERAGE(B14:B23)</f>
         <v>3.9530000000000003</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="2"/>
+      <c r="C24">
+        <f t="shared" si="4"/>
         <v>6.484</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
+      <c r="D24">
+        <f t="shared" si="4"/>
         <v>4.7410000000000005</v>
       </c>
-      <c r="E21">
-        <f t="shared" ref="E21:J21" si="3">AVERAGE(E11:E20)</f>
+      <c r="E24">
+        <f t="shared" ref="E24:J24" si="5">AVERAGE(E14:E23)</f>
         <v>3.69</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="3"/>
+      <c r="F24">
+        <f t="shared" si="5"/>
         <v>5.6109999999999989</v>
       </c>
-      <c r="G21">
-        <f t="shared" si="3"/>
+      <c r="G24">
+        <f t="shared" si="5"/>
         <v>3.6030000000000002</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="3"/>
+      <c r="H24">
+        <f t="shared" si="5"/>
         <v>1.6179999999999999</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="3"/>
+      <c r="I24">
+        <f t="shared" si="5"/>
         <v>2.42</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="3"/>
+      <c r="J24">
+        <f t="shared" si="5"/>
         <v>1.8700000000000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <f>STDEV(B11:B20)</f>
-        <v>0.98062395102981881</v>
-      </c>
-      <c r="C22">
-        <f>STDEV(C11:C20)</f>
-        <v>2.0433697658524737</v>
-      </c>
-      <c r="D22">
-        <f t="shared" ref="D22:J22" si="4">STDEV(D11:D20)</f>
-        <v>0.17181708620248193</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="4"/>
-        <v>0.11813363431112905</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="4"/>
-        <v>2.293388807468598</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="4"/>
-        <v>0.209287149894854</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="4"/>
-        <v>3.7357135269658337E-2</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="4"/>
-        <v>0.30294847380004714</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="4"/>
-        <v>2.1081851067789131E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <f>STDEV(B14:B23)</f>
+        <v>0.98062395102981881</v>
+      </c>
+      <c r="C25">
+        <f>STDEV(C14:C23)</f>
+        <v>2.0433697658524737</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:J25" si="6">STDEV(D14:D23)</f>
+        <v>0.17181708620248193</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="6"/>
+        <v>0.11813363431112905</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="6"/>
+        <v>2.293388807468598</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="6"/>
+        <v>0.209287149894854</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="6"/>
+        <v>3.7357135269658337E-2</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="6"/>
+        <v>0.30294847380004714</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="6"/>
+        <v>2.1081851067789131E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="7" t="s">
+      <c r="D28" s="8"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="I25" s="6" t="s">
+      <c r="G28" s="9"/>
+      <c r="I28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>23</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>0</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E29" t="s">
         <v>23</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F29" t="s">
         <v>0</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G29" t="s">
         <v>1</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H29" t="s">
         <v>23</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I29" t="s">
         <v>0</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J29" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <v>3.63</v>
-      </c>
-      <c r="C27">
-        <v>4.67</v>
-      </c>
-      <c r="D27">
-        <v>4.57</v>
-      </c>
-      <c r="E27">
-        <v>3.84</v>
-      </c>
-      <c r="F27">
-        <v>4.22</v>
-      </c>
-      <c r="G27">
-        <v>3.5</v>
-      </c>
-      <c r="H27">
-        <v>1.63</v>
-      </c>
-      <c r="I27">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="J27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28">
-        <v>3.48</v>
-      </c>
-      <c r="C28">
-        <v>5.08</v>
-      </c>
-      <c r="D28">
-        <v>4.74</v>
-      </c>
-      <c r="E28">
-        <v>3.7</v>
-      </c>
-      <c r="F28">
-        <v>6.27</v>
-      </c>
-      <c r="G28">
-        <v>3.8</v>
-      </c>
-      <c r="H28">
-        <v>1.63</v>
-      </c>
-      <c r="I28">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="J28">
-        <v>2.17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>3</v>
-      </c>
-      <c r="B29">
-        <v>3.56</v>
-      </c>
-      <c r="C29">
-        <v>9</v>
-      </c>
-      <c r="D29">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="E29">
-        <v>3.56</v>
-      </c>
-      <c r="F29">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G29">
-        <v>4.24</v>
-      </c>
-      <c r="H29">
-        <v>1.58</v>
-      </c>
-      <c r="I29">
-        <v>2.14</v>
-      </c>
-      <c r="J29">
-        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B30">
-        <v>3.43</v>
+        <v>3.63</v>
       </c>
       <c r="C30">
         <v>4.67</v>
       </c>
       <c r="D30">
-        <v>5.01</v>
+        <v>4.57</v>
       </c>
       <c r="E30">
-        <v>3.63</v>
+        <v>3.84</v>
       </c>
       <c r="F30">
-        <v>4.25</v>
+        <v>4.22</v>
       </c>
       <c r="G30">
-        <v>3.82</v>
+        <v>3.5</v>
       </c>
       <c r="H30">
-        <v>1.6</v>
+        <v>1.63</v>
       </c>
       <c r="I30">
-        <v>2.13</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="J30">
-        <v>2.12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B31">
-        <v>3.73</v>
+        <v>3.48</v>
       </c>
       <c r="C31">
-        <v>9.23</v>
+        <v>5.08</v>
       </c>
       <c r="D31">
-        <v>4.21</v>
+        <v>4.74</v>
       </c>
       <c r="E31">
-        <v>3.69</v>
+        <v>3.7</v>
       </c>
       <c r="F31">
-        <v>4.74</v>
+        <v>6.27</v>
       </c>
       <c r="G31">
-        <v>3.83</v>
+        <v>3.8</v>
       </c>
       <c r="H31">
-        <v>1.61</v>
+        <v>1.63</v>
       </c>
       <c r="I31">
-        <v>2.31</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="J31">
-        <v>2.16</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B32">
-        <v>3.76</v>
+        <v>3.56</v>
       </c>
       <c r="C32">
-        <v>4.26</v>
+        <v>9</v>
       </c>
       <c r="D32">
-        <v>4.46</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="E32">
-        <v>3.7</v>
+        <v>3.56</v>
       </c>
       <c r="F32">
-        <v>8.5299999999999994</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G32">
-        <v>3.72</v>
+        <v>4.24</v>
       </c>
       <c r="H32">
-        <v>1.61</v>
+        <v>1.58</v>
       </c>
       <c r="I32">
-        <v>1.89</v>
+        <v>2.14</v>
       </c>
       <c r="J32">
-        <v>2.36</v>
+        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B33">
-        <v>3.84</v>
+        <v>3.43</v>
       </c>
       <c r="C33">
-        <v>4.71</v>
+        <v>4.67</v>
       </c>
       <c r="D33">
-        <v>4.58</v>
+        <v>5.01</v>
       </c>
       <c r="E33">
-        <v>3.7</v>
+        <v>3.63</v>
       </c>
       <c r="F33">
-        <v>3.97</v>
+        <v>4.25</v>
       </c>
       <c r="G33">
-        <v>3.5</v>
+        <v>3.82</v>
       </c>
       <c r="H33">
-        <v>1.59</v>
+        <v>1.6</v>
       </c>
       <c r="I33">
-        <v>2.15</v>
+        <v>2.13</v>
       </c>
       <c r="J33">
-        <v>2.11</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B34">
-        <v>3.53</v>
+        <v>3.73</v>
       </c>
       <c r="C34">
-        <v>9.59</v>
+        <v>9.23</v>
       </c>
       <c r="D34">
-        <v>4.57</v>
+        <v>4.21</v>
       </c>
       <c r="E34">
-        <v>3.76</v>
+        <v>3.69</v>
       </c>
       <c r="F34">
-        <v>12.35</v>
+        <v>4.74</v>
       </c>
       <c r="G34">
-        <v>3.9</v>
+        <v>3.83</v>
       </c>
       <c r="H34">
-        <v>1.63</v>
+        <v>1.61</v>
       </c>
       <c r="I34">
-        <v>2.1800000000000002</v>
+        <v>2.31</v>
       </c>
       <c r="J34">
-        <v>2.1800000000000002</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B35">
-        <v>3.54</v>
+        <v>3.76</v>
       </c>
       <c r="C35">
-        <v>4.62</v>
+        <v>4.26</v>
       </c>
       <c r="D35">
-        <v>4.51</v>
+        <v>4.46</v>
       </c>
       <c r="E35">
-        <v>3.68</v>
+        <v>3.7</v>
       </c>
       <c r="F35">
-        <v>4.62</v>
+        <v>8.5299999999999994</v>
       </c>
       <c r="G35">
-        <v>3.82</v>
+        <v>3.72</v>
       </c>
       <c r="H35">
-        <v>1.62</v>
+        <v>1.61</v>
       </c>
       <c r="I35">
-        <v>3.46</v>
+        <v>1.89</v>
       </c>
       <c r="J35">
-        <v>2.33</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36">
+        <v>3.84</v>
+      </c>
+      <c r="C36">
+        <v>4.71</v>
+      </c>
+      <c r="D36">
+        <v>4.58</v>
+      </c>
+      <c r="E36">
+        <v>3.7</v>
+      </c>
+      <c r="F36">
+        <v>3.97</v>
+      </c>
+      <c r="G36">
+        <v>3.5</v>
+      </c>
+      <c r="H36">
+        <v>1.59</v>
+      </c>
+      <c r="I36">
+        <v>2.15</v>
+      </c>
+      <c r="J36">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <v>3.53</v>
+      </c>
+      <c r="C37">
+        <v>9.59</v>
+      </c>
+      <c r="D37">
+        <v>4.57</v>
+      </c>
+      <c r="E37">
+        <v>3.76</v>
+      </c>
+      <c r="F37">
+        <v>12.35</v>
+      </c>
+      <c r="G37">
+        <v>3.9</v>
+      </c>
+      <c r="H37">
+        <v>1.63</v>
+      </c>
+      <c r="I37">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="J37">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>3.54</v>
+      </c>
+      <c r="C38">
+        <v>4.62</v>
+      </c>
+      <c r="D38">
+        <v>4.51</v>
+      </c>
+      <c r="E38">
+        <v>3.68</v>
+      </c>
+      <c r="F38">
+        <v>4.62</v>
+      </c>
+      <c r="G38">
+        <v>3.82</v>
+      </c>
+      <c r="H38">
+        <v>1.62</v>
+      </c>
+      <c r="I38">
+        <v>3.46</v>
+      </c>
+      <c r="J38">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>10</v>
       </c>
-      <c r="B36">
+      <c r="B39">
         <v>3.57</v>
       </c>
-      <c r="C36">
+      <c r="C39">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D36">
+      <c r="D39">
         <v>4.71</v>
       </c>
-      <c r="E36">
+      <c r="E39">
         <v>3.76</v>
       </c>
-      <c r="F36">
+      <c r="F39">
         <v>4.26</v>
       </c>
-      <c r="G36">
+      <c r="G39">
         <v>3.59</v>
       </c>
-      <c r="H36">
+      <c r="H39">
         <v>1.63</v>
       </c>
-      <c r="I36">
+      <c r="I39">
         <v>2.6</v>
       </c>
-      <c r="J36">
+      <c r="J39">
         <v>2.13</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>3</v>
       </c>
-      <c r="B37">
-        <f t="shared" ref="B37:D37" si="5">AVERAGE(B27:B36)</f>
+      <c r="B40">
+        <f t="shared" ref="B40:D40" si="7">AVERAGE(B30:B39)</f>
         <v>3.6070000000000002</v>
       </c>
-      <c r="C37">
-        <f t="shared" si="5"/>
+      <c r="C40">
+        <f t="shared" si="7"/>
         <v>6.043000000000001</v>
       </c>
-      <c r="D37">
-        <f t="shared" si="5"/>
+      <c r="D40">
+        <f t="shared" si="7"/>
         <v>4.5840000000000005</v>
       </c>
-      <c r="E37">
-        <f t="shared" ref="E37:G37" si="6">AVERAGE(E27:E36)</f>
+      <c r="E40">
+        <f t="shared" ref="E40:G40" si="8">AVERAGE(E30:E39)</f>
         <v>3.7019999999999995</v>
       </c>
-      <c r="F37">
-        <f t="shared" si="6"/>
+      <c r="F40">
+        <f t="shared" si="8"/>
         <v>5.8109999999999999</v>
       </c>
-      <c r="G37">
-        <f t="shared" si="6"/>
+      <c r="G40">
+        <f t="shared" si="8"/>
         <v>3.7719999999999998</v>
       </c>
-      <c r="H37">
-        <f t="shared" ref="H37:J37" si="7">AVERAGE(H27:H36)</f>
+      <c r="H40">
+        <f t="shared" ref="H40:J40" si="9">AVERAGE(H30:H39)</f>
         <v>1.613</v>
       </c>
-      <c r="I37">
-        <f t="shared" si="7"/>
+      <c r="I40">
+        <f t="shared" si="9"/>
         <v>2.3610000000000002</v>
       </c>
-      <c r="J37">
-        <f t="shared" si="7"/>
+      <c r="J40">
+        <f t="shared" si="9"/>
         <v>2.1879999999999997</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38">
-        <f>STDEV(B27:B36)</f>
-        <v>0.13115300648902831</v>
-      </c>
-      <c r="C38">
-        <f>STDEV(C27:C36)</f>
-        <v>2.2420925246048329</v>
-      </c>
-      <c r="D38">
-        <f t="shared" ref="D38" si="8">STDEV(D27:D36)</f>
-        <v>0.2091357878933631</v>
-      </c>
-      <c r="E38">
-        <f t="shared" ref="E38:G38" si="9">STDEV(E27:E36)</f>
-        <v>7.5836080536319267E-2</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="9"/>
-        <v>2.6774882508301197</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="9"/>
-        <v>0.21806217258183763</v>
-      </c>
-      <c r="H38">
-        <f t="shared" ref="H38:J38" si="10">STDEV(H27:H36)</f>
-        <v>1.8287822299126861E-2</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="10"/>
-        <v>0.43534022454984561</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="10"/>
-        <v>0.11438725647747847</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <f>STDEV(B30:B39)</f>
+        <v>0.13115300648902831</v>
+      </c>
+      <c r="C41">
+        <f>STDEV(C30:C39)</f>
+        <v>2.2420925246048329</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ref="D41" si="10">STDEV(D30:D39)</f>
+        <v>0.2091357878933631</v>
+      </c>
+      <c r="E41">
+        <f t="shared" ref="E41:G41" si="11">STDEV(E30:E39)</f>
+        <v>7.5836080536319267E-2</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="11"/>
+        <v>2.6774882508301197</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="11"/>
+        <v>0.21806217258183763</v>
+      </c>
+      <c r="H41">
+        <f t="shared" ref="H41:J41" si="12">STDEV(H30:H39)</f>
+        <v>1.8287822299126861E-2</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="12"/>
+        <v>0.43534022454984561</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="12"/>
+        <v>0.11438725647747847</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C44" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="7" t="s">
+      <c r="D44" s="8"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G41" s="7"/>
-      <c r="I41" s="6" t="s">
+      <c r="G44" s="9"/>
+      <c r="I44" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="J44" s="8"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>23</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C45" t="s">
         <v>0</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D45" t="s">
         <v>1</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E45" t="s">
         <v>23</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F45" t="s">
         <v>0</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G45" t="s">
         <v>1</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H45" t="s">
         <v>23</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I45" t="s">
         <v>0</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J45" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43">
-        <v>3.54</v>
-      </c>
-      <c r="C43">
-        <v>7.88</v>
-      </c>
-      <c r="D43">
-        <v>4.59</v>
-      </c>
-      <c r="E43">
-        <v>3.79</v>
-      </c>
-      <c r="F43">
-        <v>4.21</v>
-      </c>
-      <c r="G43">
-        <v>3.8</v>
-      </c>
-      <c r="H43">
-        <v>1.62</v>
-      </c>
-      <c r="I43">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J43">
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>2</v>
-      </c>
-      <c r="B44">
-        <v>3.87</v>
-      </c>
-      <c r="C44">
-        <v>4.54</v>
-      </c>
-      <c r="D44">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="E44">
-        <v>3.78</v>
-      </c>
-      <c r="F44">
-        <v>4.49</v>
-      </c>
-      <c r="G44">
-        <v>4.03</v>
-      </c>
-      <c r="H44">
-        <v>1.66</v>
-      </c>
-      <c r="I44">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="J44">
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>3</v>
-      </c>
-      <c r="B45">
-        <v>3.84</v>
-      </c>
-      <c r="C45">
-        <v>8.35</v>
-      </c>
-      <c r="D45">
-        <v>4.72</v>
-      </c>
-      <c r="E45">
-        <v>3.76</v>
-      </c>
-      <c r="F45">
-        <v>9.8699999999999992</v>
-      </c>
-      <c r="G45">
-        <v>3.88</v>
-      </c>
-      <c r="H45">
-        <v>1.59</v>
-      </c>
-      <c r="I45">
-        <v>1.96</v>
-      </c>
-      <c r="J45">
-        <v>1.74</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B46">
-        <v>3.61</v>
+        <v>3.54</v>
       </c>
       <c r="C46">
-        <v>4.5</v>
+        <v>7.88</v>
       </c>
       <c r="D46">
-        <v>4.79</v>
+        <v>4.59</v>
       </c>
       <c r="E46">
-        <v>3.64</v>
+        <v>3.79</v>
       </c>
       <c r="F46">
-        <v>4.66</v>
+        <v>4.21</v>
       </c>
       <c r="G46">
-        <v>3.54</v>
+        <v>3.8</v>
       </c>
       <c r="H46">
-        <v>1.6</v>
+        <v>1.62</v>
       </c>
       <c r="I46">
-        <v>2.1800000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="J46">
-        <v>1.76</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B47">
-        <v>4.1399999999999997</v>
+        <v>3.87</v>
       </c>
       <c r="C47">
-        <v>4.67</v>
+        <v>4.54</v>
       </c>
       <c r="D47">
-        <v>4.53</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="E47">
-        <v>3.72</v>
+        <v>3.78</v>
       </c>
       <c r="F47">
-        <v>4.6399999999999997</v>
+        <v>4.49</v>
       </c>
       <c r="G47">
-        <v>4.8600000000000003</v>
+        <v>4.03</v>
       </c>
       <c r="H47">
-        <v>1.59</v>
+        <v>1.66</v>
       </c>
       <c r="I47">
-        <v>2.16</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="J47">
-        <v>1.78</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B48">
-        <v>3.64</v>
+        <v>3.84</v>
       </c>
       <c r="C48">
-        <v>7.88</v>
+        <v>8.35</v>
       </c>
       <c r="D48">
-        <v>4.6100000000000003</v>
+        <v>4.72</v>
       </c>
       <c r="E48">
-        <v>3.86</v>
+        <v>3.76</v>
       </c>
       <c r="F48">
-        <v>4.7300000000000004</v>
+        <v>9.8699999999999992</v>
       </c>
       <c r="G48">
-        <v>3.58</v>
+        <v>3.88</v>
       </c>
       <c r="H48">
-        <v>1.55</v>
+        <v>1.59</v>
       </c>
       <c r="I48">
-        <v>1.87</v>
+        <v>1.96</v>
       </c>
       <c r="J48">
-        <v>2.4500000000000002</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B49">
-        <v>3.41</v>
+        <v>3.61</v>
       </c>
       <c r="C49">
-        <v>4.0599999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="D49">
-        <v>4.13</v>
+        <v>4.79</v>
       </c>
       <c r="E49">
-        <v>3.89</v>
+        <v>3.64</v>
       </c>
       <c r="F49">
-        <v>4.45</v>
+        <v>4.66</v>
       </c>
       <c r="G49">
-        <v>3.74</v>
+        <v>3.54</v>
       </c>
       <c r="H49">
-        <v>1.58</v>
+        <v>1.6</v>
       </c>
       <c r="I49">
-        <v>2.99</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="J49">
-        <v>2.21</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B50">
-        <v>4.07</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="C50">
-        <v>4.75</v>
+        <v>4.67</v>
       </c>
       <c r="D50">
-        <v>4.58</v>
+        <v>4.53</v>
       </c>
       <c r="E50">
-        <v>3.75</v>
+        <v>3.72</v>
       </c>
       <c r="F50">
-        <v>8.39</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="G50">
-        <v>3.56</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="H50">
         <v>1.59</v>
       </c>
       <c r="I50">
-        <v>3.33</v>
+        <v>2.16</v>
       </c>
       <c r="J50">
-        <v>1.8</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B51">
-        <v>4.12</v>
+        <v>3.64</v>
       </c>
       <c r="C51">
-        <v>9.5299999999999994</v>
+        <v>7.88</v>
       </c>
       <c r="D51">
-        <v>4.68</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="E51">
-        <v>3.75</v>
+        <v>3.86</v>
       </c>
       <c r="F51">
-        <v>4.46</v>
+        <v>4.7300000000000004</v>
       </c>
       <c r="G51">
-        <v>3.71</v>
+        <v>3.58</v>
       </c>
       <c r="H51">
-        <v>1.61</v>
+        <v>1.55</v>
       </c>
       <c r="I51">
-        <v>1.92</v>
+        <v>1.87</v>
       </c>
       <c r="J51">
-        <v>1.81</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
+        <v>7</v>
+      </c>
+      <c r="B52">
+        <v>3.41</v>
+      </c>
+      <c r="C52">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="D52">
+        <v>4.13</v>
+      </c>
+      <c r="E52">
+        <v>3.89</v>
+      </c>
+      <c r="F52">
+        <v>4.45</v>
+      </c>
+      <c r="G52">
+        <v>3.74</v>
+      </c>
+      <c r="H52">
+        <v>1.58</v>
+      </c>
+      <c r="I52">
+        <v>2.99</v>
+      </c>
+      <c r="J52">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>8</v>
+      </c>
+      <c r="B53">
+        <v>4.07</v>
+      </c>
+      <c r="C53">
+        <v>4.75</v>
+      </c>
+      <c r="D53">
+        <v>4.58</v>
+      </c>
+      <c r="E53">
+        <v>3.75</v>
+      </c>
+      <c r="F53">
+        <v>8.39</v>
+      </c>
+      <c r="G53">
+        <v>3.56</v>
+      </c>
+      <c r="H53">
+        <v>1.59</v>
+      </c>
+      <c r="I53">
+        <v>3.33</v>
+      </c>
+      <c r="J53">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>9</v>
+      </c>
+      <c r="B54">
+        <v>4.12</v>
+      </c>
+      <c r="C54">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="D54">
+        <v>4.68</v>
+      </c>
+      <c r="E54">
+        <v>3.75</v>
+      </c>
+      <c r="F54">
+        <v>4.46</v>
+      </c>
+      <c r="G54">
+        <v>3.71</v>
+      </c>
+      <c r="H54">
+        <v>1.61</v>
+      </c>
+      <c r="I54">
+        <v>1.92</v>
+      </c>
+      <c r="J54">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>10</v>
       </c>
-      <c r="B52">
+      <c r="B55">
         <v>3.61</v>
       </c>
-      <c r="C52">
+      <c r="C55">
         <v>8.4499999999999993</v>
       </c>
-      <c r="D52">
+      <c r="D55">
         <v>4.4800000000000004</v>
       </c>
-      <c r="E52">
+      <c r="E55">
         <v>4.25</v>
       </c>
-      <c r="F52">
+      <c r="F55">
         <v>3.91</v>
       </c>
-      <c r="G52">
+      <c r="G55">
         <v>3.64</v>
       </c>
-      <c r="H52">
+      <c r="H55">
         <v>1.6</v>
       </c>
-      <c r="I52">
+      <c r="I55">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J52">
+      <c r="J55">
         <v>2.02</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>3</v>
       </c>
-      <c r="B53">
-        <f t="shared" ref="B53:D53" si="11">AVERAGE(B43:B52)</f>
+      <c r="B56">
+        <f t="shared" ref="B56:D56" si="13">AVERAGE(B46:B55)</f>
         <v>3.7850000000000001</v>
       </c>
-      <c r="C53">
-        <f t="shared" si="11"/>
+      <c r="C56">
+        <f t="shared" si="13"/>
         <v>6.4610000000000003</v>
       </c>
-      <c r="D53">
-        <f t="shared" si="11"/>
+      <c r="D56">
+        <f t="shared" si="13"/>
         <v>4.55</v>
       </c>
-      <c r="E53">
-        <f t="shared" ref="E53:G53" si="12">AVERAGE(E43:E52)</f>
+      <c r="E56">
+        <f t="shared" ref="E56:G56" si="14">AVERAGE(E46:E55)</f>
         <v>3.819</v>
       </c>
-      <c r="F53">
-        <f t="shared" si="12"/>
+      <c r="F56">
+        <f t="shared" si="14"/>
         <v>5.3810000000000002</v>
       </c>
-      <c r="G53">
-        <f t="shared" si="12"/>
+      <c r="G56">
+        <f t="shared" si="14"/>
         <v>3.8339999999999996</v>
       </c>
-      <c r="H53">
-        <f t="shared" ref="H53:J53" si="13">AVERAGE(H43:H52)</f>
+      <c r="H56">
+        <f t="shared" ref="H56:J56" si="15">AVERAGE(H46:H55)</f>
         <v>1.599</v>
       </c>
-      <c r="I53">
-        <f t="shared" si="13"/>
+      <c r="I56">
+        <f t="shared" si="15"/>
         <v>2.3090000000000002</v>
       </c>
-      <c r="J53">
-        <f t="shared" si="13"/>
+      <c r="J56">
+        <f t="shared" si="15"/>
         <v>1.921</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54">
-        <f>STDEV(B43:B52)</f>
-        <v>0.26090653924772034</v>
-      </c>
-      <c r="C54">
-        <f>STDEV(C43:C52)</f>
-        <v>2.1188594940570149</v>
-      </c>
-      <c r="D54">
-        <f t="shared" ref="D54" si="14">STDEV(D43:D52)</f>
-        <v>0.18761663039293719</v>
-      </c>
-      <c r="E54">
-        <f t="shared" ref="E54:G54" si="15">STDEV(E43:E52)</f>
-        <v>0.16656330128012392</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="15"/>
-        <v>2.0205029626858302</v>
-      </c>
-      <c r="G54">
-        <f t="shared" si="15"/>
-        <v>0.39189567772842593</v>
-      </c>
-      <c r="H54">
-        <f t="shared" ref="H54:J54" si="16">STDEV(H43:H52)</f>
-        <v>2.8460498941515384E-2</v>
-      </c>
-      <c r="I54">
-        <f t="shared" si="16"/>
-        <v>0.47603571294599406</v>
-      </c>
-      <c r="J54">
-        <f t="shared" si="16"/>
-        <v>0.23718019403913904</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57">
+        <f>STDEV(B46:B55)</f>
+        <v>0.26090653924772034</v>
+      </c>
+      <c r="C57">
+        <f>STDEV(C46:C55)</f>
+        <v>2.1188594940570149</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ref="D57" si="16">STDEV(D46:D55)</f>
+        <v>0.18761663039293719</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ref="E57:G57" si="17">STDEV(E46:E55)</f>
+        <v>0.16656330128012392</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="17"/>
+        <v>2.0205029626858302</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="17"/>
+        <v>0.39189567772842593</v>
+      </c>
+      <c r="H57">
+        <f t="shared" ref="H57:J57" si="18">STDEV(H46:H55)</f>
+        <v>2.8460498941515384E-2</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="18"/>
+        <v>0.47603571294599406</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="18"/>
+        <v>0.23718019403913904</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C60" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="7" t="s">
+      <c r="D60" s="8"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="7"/>
-      <c r="I57" s="6" t="s">
+      <c r="G60" s="9"/>
+      <c r="I60" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J57" s="6"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="J60" s="8"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>23</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C61" t="s">
         <v>0</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D61" t="s">
         <v>1</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E61" t="s">
         <v>23</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F61" t="s">
         <v>0</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G61" t="s">
         <v>1</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H61" t="s">
         <v>23</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I61" t="s">
         <v>0</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J61" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>1</v>
-      </c>
-      <c r="B59">
-        <v>3.46</v>
-      </c>
-      <c r="C59">
-        <v>3.86</v>
-      </c>
-      <c r="D59">
-        <v>4.5</v>
-      </c>
-      <c r="E59">
-        <v>3.84</v>
-      </c>
-      <c r="F59">
-        <v>5.07</v>
-      </c>
-      <c r="G59">
-        <v>3.88</v>
-      </c>
-      <c r="H59">
-        <v>1.6</v>
-      </c>
-      <c r="I59">
-        <v>2.31</v>
-      </c>
-      <c r="J59">
-        <v>1.81</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>2</v>
-      </c>
-      <c r="B60">
-        <v>3.35</v>
-      </c>
-      <c r="C60">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="D60">
-        <v>4.78</v>
-      </c>
-      <c r="E60">
-        <v>3.8</v>
-      </c>
-      <c r="F60">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="G60">
-        <v>3.85</v>
-      </c>
-      <c r="H60">
-        <v>1.58</v>
-      </c>
-      <c r="I60">
-        <v>2.09</v>
-      </c>
-      <c r="J60">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>3</v>
-      </c>
-      <c r="B61">
-        <v>3.63</v>
-      </c>
-      <c r="C61">
-        <v>5.34</v>
-      </c>
-      <c r="D61">
-        <v>4.38</v>
-      </c>
-      <c r="E61">
-        <v>3.73</v>
-      </c>
-      <c r="F61">
-        <v>3.68</v>
-      </c>
-      <c r="G61">
-        <v>4.08</v>
-      </c>
-      <c r="H61">
-        <v>1.64</v>
-      </c>
-      <c r="I61">
-        <v>1.97</v>
-      </c>
-      <c r="J61">
-        <v>1.84</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B62">
-        <v>3.85</v>
+        <v>3.46</v>
       </c>
       <c r="C62">
-        <v>4.88</v>
+        <v>3.86</v>
       </c>
       <c r="D62">
-        <v>4.9400000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="E62">
-        <v>3.43</v>
+        <v>3.84</v>
       </c>
       <c r="F62">
-        <v>4.1900000000000004</v>
+        <v>5.07</v>
       </c>
       <c r="G62">
-        <v>3.7</v>
+        <v>3.88</v>
       </c>
       <c r="H62">
-        <v>1.59</v>
+        <v>1.6</v>
       </c>
       <c r="I62">
-        <v>2.1</v>
+        <v>2.31</v>
       </c>
       <c r="J62">
-        <v>1.85</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B63">
-        <v>4.04</v>
+        <v>3.35</v>
       </c>
       <c r="C63">
-        <v>4.07</v>
-      </c>
-      <c r="D63" t="s">
-        <v>21</v>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="D63">
+        <v>4.78</v>
       </c>
       <c r="E63">
-        <v>3.65</v>
+        <v>3.8</v>
       </c>
       <c r="F63">
-        <v>4.42</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="G63">
-        <v>3.56</v>
+        <v>3.85</v>
       </c>
       <c r="H63">
-        <v>1.6</v>
+        <v>1.58</v>
       </c>
       <c r="I63">
-        <v>2.6</v>
+        <v>2.09</v>
       </c>
       <c r="J63">
-        <v>1.82</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B64">
-        <v>3.43</v>
+        <v>3.63</v>
       </c>
       <c r="C64">
-        <v>9.5399999999999991</v>
+        <v>5.34</v>
       </c>
       <c r="D64">
-        <v>4.58</v>
+        <v>4.38</v>
       </c>
       <c r="E64">
-        <v>3.75</v>
+        <v>3.73</v>
       </c>
       <c r="F64">
-        <v>3.9</v>
+        <v>3.68</v>
       </c>
       <c r="G64">
-        <v>4.05</v>
+        <v>4.08</v>
       </c>
       <c r="H64">
-        <v>1.57</v>
+        <v>1.64</v>
       </c>
       <c r="I64">
-        <v>2.67</v>
+        <v>1.97</v>
       </c>
       <c r="J64">
-        <v>1.87</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B65">
-        <v>3.76</v>
+        <v>3.85</v>
       </c>
       <c r="C65">
-        <v>4.82</v>
+        <v>4.88</v>
       </c>
       <c r="D65">
-        <v>4.6500000000000004</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="E65">
-        <v>3.85</v>
+        <v>3.43</v>
       </c>
       <c r="F65">
-        <v>4.63</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="G65">
-        <v>3.67</v>
+        <v>3.7</v>
       </c>
       <c r="H65">
-        <v>1.58</v>
+        <v>1.59</v>
       </c>
       <c r="I65">
-        <v>2.13</v>
+        <v>2.1</v>
       </c>
       <c r="J65">
-        <v>1.75</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B66">
-        <v>3.46</v>
+        <v>4.04</v>
       </c>
       <c r="C66">
-        <v>8.11</v>
-      </c>
-      <c r="D66">
-        <v>4.32</v>
+        <v>4.07</v>
+      </c>
+      <c r="D66" t="s">
+        <v>21</v>
       </c>
       <c r="E66">
-        <v>3.49</v>
+        <v>3.65</v>
       </c>
       <c r="F66">
-        <v>4.53</v>
+        <v>4.42</v>
       </c>
       <c r="G66">
-        <v>3.53</v>
+        <v>3.56</v>
       </c>
       <c r="H66">
-        <v>1.59</v>
+        <v>1.6</v>
       </c>
       <c r="I66">
-        <v>2.0699999999999998</v>
+        <v>2.6</v>
       </c>
       <c r="J66">
-        <v>1.83</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B67">
-        <v>3.56</v>
+        <v>3.43</v>
       </c>
       <c r="C67">
-        <v>4.16</v>
+        <v>9.5399999999999991</v>
       </c>
       <c r="D67">
-        <v>4.57</v>
+        <v>4.58</v>
       </c>
       <c r="E67">
-        <v>3.85</v>
+        <v>3.75</v>
       </c>
       <c r="F67">
-        <v>3.75</v>
+        <v>3.9</v>
       </c>
       <c r="G67">
-        <v>3.68</v>
+        <v>4.05</v>
       </c>
       <c r="H67">
-        <v>1.59</v>
+        <v>1.57</v>
       </c>
       <c r="I67">
-        <v>2.04</v>
+        <v>2.67</v>
       </c>
       <c r="J67">
-        <v>1.8</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
+        <v>7</v>
+      </c>
+      <c r="B68">
+        <v>3.76</v>
+      </c>
+      <c r="C68">
+        <v>4.82</v>
+      </c>
+      <c r="D68">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="E68">
+        <v>3.85</v>
+      </c>
+      <c r="F68">
+        <v>4.63</v>
+      </c>
+      <c r="G68">
+        <v>3.67</v>
+      </c>
+      <c r="H68">
+        <v>1.58</v>
+      </c>
+      <c r="I68">
+        <v>2.13</v>
+      </c>
+      <c r="J68">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>8</v>
+      </c>
+      <c r="B69">
+        <v>3.46</v>
+      </c>
+      <c r="C69">
+        <v>8.11</v>
+      </c>
+      <c r="D69">
+        <v>4.32</v>
+      </c>
+      <c r="E69">
+        <v>3.49</v>
+      </c>
+      <c r="F69">
+        <v>4.53</v>
+      </c>
+      <c r="G69">
+        <v>3.53</v>
+      </c>
+      <c r="H69">
+        <v>1.59</v>
+      </c>
+      <c r="I69">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="J69">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>9</v>
+      </c>
+      <c r="B70">
+        <v>3.56</v>
+      </c>
+      <c r="C70">
+        <v>4.16</v>
+      </c>
+      <c r="D70">
+        <v>4.57</v>
+      </c>
+      <c r="E70">
+        <v>3.85</v>
+      </c>
+      <c r="F70">
+        <v>3.75</v>
+      </c>
+      <c r="G70">
+        <v>3.68</v>
+      </c>
+      <c r="H70">
+        <v>1.59</v>
+      </c>
+      <c r="I70">
+        <v>2.04</v>
+      </c>
+      <c r="J70">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>10</v>
       </c>
-      <c r="B68">
+      <c r="B71">
         <v>3.34</v>
       </c>
-      <c r="C68">
+      <c r="C71">
         <v>8.44</v>
       </c>
-      <c r="D68">
+      <c r="D71">
         <v>4.7699999999999996</v>
       </c>
-      <c r="E68">
+      <c r="E71">
         <v>3.71</v>
       </c>
-      <c r="F68">
+      <c r="F71">
         <v>4.75</v>
       </c>
-      <c r="G68">
+      <c r="G71">
         <v>3.66</v>
       </c>
-      <c r="H68">
+      <c r="H71">
         <v>1.59</v>
       </c>
-      <c r="I68">
+      <c r="I71">
         <v>2.37</v>
       </c>
-      <c r="J68">
+      <c r="J71">
         <v>1.84</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>3</v>
       </c>
-      <c r="B69">
-        <f t="shared" ref="B69:D69" si="17">AVERAGE(B59:B68)</f>
+      <c r="B72">
+        <f t="shared" ref="B72:D72" si="19">AVERAGE(B62:B71)</f>
         <v>3.588000000000001</v>
       </c>
-      <c r="C69">
-        <f t="shared" si="17"/>
+      <c r="C72">
+        <f t="shared" si="19"/>
         <v>5.7329999999999997</v>
       </c>
-      <c r="D69">
-        <f t="shared" si="17"/>
+      <c r="D72">
+        <f t="shared" si="19"/>
         <v>4.6099999999999994</v>
       </c>
-      <c r="E69">
-        <f t="shared" ref="E69:G69" si="18">AVERAGE(E59:E68)</f>
+      <c r="E72">
+        <f t="shared" ref="E72:G72" si="20">AVERAGE(E62:E71)</f>
         <v>3.71</v>
       </c>
-      <c r="F69">
-        <f t="shared" si="18"/>
+      <c r="F72">
+        <f t="shared" si="20"/>
         <v>4.3309999999999995</v>
       </c>
-      <c r="G69">
-        <f t="shared" si="18"/>
+      <c r="G72">
+        <f t="shared" si="20"/>
         <v>3.7659999999999996</v>
       </c>
-      <c r="H69">
-        <f t="shared" ref="H69:J69" si="19">AVERAGE(H59:H68)</f>
+      <c r="H72">
+        <f t="shared" ref="H72:J72" si="21">AVERAGE(H62:H71)</f>
         <v>1.593</v>
       </c>
-      <c r="I69">
-        <f t="shared" si="19"/>
+      <c r="I72">
+        <f t="shared" si="21"/>
         <v>2.2350000000000003</v>
       </c>
-      <c r="J69">
-        <f t="shared" si="19"/>
+      <c r="J72">
+        <f t="shared" si="21"/>
         <v>1.8559999999999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>7</v>
-      </c>
-      <c r="B70">
-        <f>STDEV(B59:B68)</f>
-        <v>0.23117093242879824</v>
-      </c>
-      <c r="C70">
-        <f>STDEV(C59:C68)</f>
-        <v>2.1231268868764728</v>
-      </c>
-      <c r="D70">
-        <f t="shared" ref="D70" si="20">STDEV(D59:D68)</f>
-        <v>0.19893466264077764</v>
-      </c>
-      <c r="E70">
-        <f t="shared" ref="E70:G70" si="21">STDEV(E59:E68)</f>
-        <v>0.14779866184930235</v>
-      </c>
-      <c r="F70">
-        <f t="shared" si="21"/>
-        <v>0.45081284611490635</v>
-      </c>
-      <c r="G70">
-        <f t="shared" si="21"/>
-        <v>0.19138094645671147</v>
-      </c>
-      <c r="H70">
-        <f t="shared" ref="H70:J70" si="22">STDEV(H59:H68)</f>
-        <v>1.8885620632287017E-2</v>
-      </c>
-      <c r="I70">
-        <f t="shared" si="22"/>
-        <v>0.24313919195939279</v>
-      </c>
-      <c r="J70">
-        <f t="shared" si="22"/>
-        <v>0.10834102536794532</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73">
+        <f>STDEV(B62:B71)</f>
+        <v>0.23117093242879824</v>
+      </c>
+      <c r="C73">
+        <f>STDEV(C62:C71)</f>
+        <v>2.1231268868764728</v>
+      </c>
+      <c r="D73">
+        <f t="shared" ref="D73" si="22">STDEV(D62:D71)</f>
+        <v>0.19893466264077764</v>
+      </c>
+      <c r="E73">
+        <f t="shared" ref="E73:G73" si="23">STDEV(E62:E71)</f>
+        <v>0.14779866184930235</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="23"/>
+        <v>0.45081284611490635</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="23"/>
+        <v>0.19138094645671147</v>
+      </c>
+      <c r="H73">
+        <f t="shared" ref="H73:J73" si="24">STDEV(H62:H71)</f>
+        <v>1.8885620632287017E-2</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="24"/>
+        <v>0.24313919195939279</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="24"/>
+        <v>0.10834102536794532</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C76" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D73" s="6"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="7" t="s">
+      <c r="D76" s="8"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G73" s="7"/>
-      <c r="I73" s="6" t="s">
+      <c r="G76" s="9"/>
+      <c r="I76" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J73" s="6"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="J76" s="8"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>23</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C77" t="s">
         <v>0</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D77" t="s">
         <v>1</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E77" t="s">
         <v>23</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F77" t="s">
         <v>0</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G77" t="s">
         <v>1</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H77" t="s">
         <v>23</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I77" t="s">
         <v>0</v>
       </c>
-      <c r="J74" t="s">
+      <c r="J77" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>1</v>
-      </c>
-      <c r="B75">
-        <v>3.59</v>
-      </c>
-      <c r="C75">
-        <v>4.95</v>
-      </c>
-      <c r="D75">
-        <v>4.96</v>
-      </c>
-      <c r="E75">
-        <v>3.83</v>
-      </c>
-      <c r="F75">
-        <v>3.46</v>
-      </c>
-      <c r="G75">
-        <v>3.61</v>
-      </c>
-      <c r="H75">
-        <v>1.58</v>
-      </c>
-      <c r="I75">
-        <v>1.8</v>
-      </c>
-      <c r="J75">
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>2</v>
-      </c>
-      <c r="B76">
-        <v>3.66</v>
-      </c>
-      <c r="C76">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="D76">
-        <v>4.7</v>
-      </c>
-      <c r="E76">
-        <v>3.72</v>
-      </c>
-      <c r="F76">
-        <v>4.8600000000000003</v>
-      </c>
-      <c r="G76">
-        <v>3.62</v>
-      </c>
-      <c r="H76">
-        <v>1.61</v>
-      </c>
-      <c r="I76">
-        <v>1.8</v>
-      </c>
-      <c r="J76">
-        <v>2.08</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>3</v>
-      </c>
-      <c r="B77">
-        <v>3.33</v>
-      </c>
-      <c r="C77">
-        <v>8.34</v>
-      </c>
-      <c r="D77">
-        <v>4.74</v>
-      </c>
-      <c r="E77">
-        <v>3.76</v>
-      </c>
-      <c r="F77">
-        <v>3.64</v>
-      </c>
-      <c r="G77">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="H77">
-        <v>1.61</v>
-      </c>
-      <c r="I77">
-        <v>2.8</v>
-      </c>
-      <c r="J77">
-        <v>1.86</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B78">
-        <v>3.63</v>
+        <v>3.59</v>
       </c>
       <c r="C78">
-        <v>4.84</v>
+        <v>4.95</v>
       </c>
       <c r="D78">
-        <v>4.57</v>
+        <v>4.96</v>
       </c>
       <c r="E78">
-        <v>3.88</v>
+        <v>3.83</v>
       </c>
       <c r="F78">
-        <v>4.1399999999999997</v>
+        <v>3.46</v>
       </c>
       <c r="G78">
-        <v>3.62</v>
+        <v>3.61</v>
       </c>
       <c r="H78">
-        <v>1.65</v>
+        <v>1.58</v>
       </c>
       <c r="I78">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="J78">
-        <v>1.73</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B79">
-        <v>3.42</v>
+        <v>3.66</v>
       </c>
       <c r="C79">
-        <v>4.68</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="D79">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="E79">
-        <v>3.7</v>
+        <v>3.72</v>
       </c>
       <c r="F79">
-        <v>4.67</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="G79">
-        <v>4.01</v>
+        <v>3.62</v>
       </c>
       <c r="H79">
-        <v>1.63</v>
+        <v>1.61</v>
       </c>
       <c r="I79">
-        <v>2.29</v>
+        <v>1.8</v>
       </c>
       <c r="J79">
-        <v>1.74</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B80">
-        <v>3.64</v>
+        <v>3.33</v>
       </c>
       <c r="C80">
-        <v>4.07</v>
+        <v>8.34</v>
       </c>
       <c r="D80">
-        <v>4.84</v>
+        <v>4.74</v>
       </c>
       <c r="E80">
         <v>3.76</v>
       </c>
       <c r="F80">
-        <v>3.91</v>
+        <v>3.64</v>
       </c>
       <c r="G80">
-        <v>4</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="H80">
-        <v>1.6</v>
+        <v>1.61</v>
       </c>
       <c r="I80">
-        <v>2.48</v>
+        <v>2.8</v>
       </c>
       <c r="J80">
-        <v>1.77</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B81">
-        <v>3.55</v>
+        <v>3.63</v>
       </c>
       <c r="C81">
-        <v>4.33</v>
+        <v>4.84</v>
       </c>
       <c r="D81">
-        <v>4.6399999999999997</v>
+        <v>4.57</v>
       </c>
       <c r="E81">
-        <v>3.68</v>
+        <v>3.88</v>
       </c>
       <c r="F81">
-        <v>4.13</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="G81">
-        <v>3.8</v>
+        <v>3.62</v>
       </c>
       <c r="H81">
-        <v>1.57</v>
+        <v>1.65</v>
       </c>
       <c r="I81">
         <v>1.75</v>
       </c>
       <c r="J81">
-        <v>1.79</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B82">
-        <v>3.47</v>
+        <v>3.42</v>
       </c>
       <c r="C82">
-        <v>4.7300000000000004</v>
+        <v>4.68</v>
       </c>
       <c r="D82">
-        <v>4.75</v>
+        <v>4.8</v>
       </c>
       <c r="E82">
         <v>3.7</v>
       </c>
       <c r="F82">
-        <v>5.14</v>
+        <v>4.67</v>
       </c>
       <c r="G82">
-        <v>3.59</v>
+        <v>4.01</v>
       </c>
       <c r="H82">
-        <v>1.6</v>
+        <v>1.63</v>
       </c>
       <c r="I82">
-        <v>1.78</v>
+        <v>2.29</v>
       </c>
       <c r="J82">
-        <v>1.82</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B83">
-        <v>3.63</v>
+        <v>3.64</v>
       </c>
       <c r="C83">
-        <v>8.4600000000000009</v>
+        <v>4.07</v>
       </c>
       <c r="D83">
-        <v>4.5999999999999996</v>
+        <v>4.84</v>
       </c>
       <c r="E83">
         <v>3.76</v>
       </c>
       <c r="F83">
-        <v>3.88</v>
+        <v>3.91</v>
       </c>
       <c r="G83">
-        <v>4.3600000000000003</v>
+        <v>4</v>
       </c>
       <c r="H83">
         <v>1.6</v>
       </c>
       <c r="I83">
-        <v>2.11</v>
+        <v>2.48</v>
       </c>
       <c r="J83">
-        <v>1.75</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
+        <v>7</v>
+      </c>
+      <c r="B84">
+        <v>3.55</v>
+      </c>
+      <c r="C84">
+        <v>4.33</v>
+      </c>
+      <c r="D84">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="E84">
+        <v>3.68</v>
+      </c>
+      <c r="F84">
+        <v>4.13</v>
+      </c>
+      <c r="G84">
+        <v>3.8</v>
+      </c>
+      <c r="H84">
+        <v>1.57</v>
+      </c>
+      <c r="I84">
+        <v>1.75</v>
+      </c>
+      <c r="J84">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>8</v>
+      </c>
+      <c r="B85">
+        <v>3.47</v>
+      </c>
+      <c r="C85">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="D85">
+        <v>4.75</v>
+      </c>
+      <c r="E85">
+        <v>3.7</v>
+      </c>
+      <c r="F85">
+        <v>5.14</v>
+      </c>
+      <c r="G85">
+        <v>3.59</v>
+      </c>
+      <c r="H85">
+        <v>1.6</v>
+      </c>
+      <c r="I85">
+        <v>1.78</v>
+      </c>
+      <c r="J85">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>9</v>
+      </c>
+      <c r="B86">
+        <v>3.63</v>
+      </c>
+      <c r="C86">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="D86">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E86">
+        <v>3.76</v>
+      </c>
+      <c r="F86">
+        <v>3.88</v>
+      </c>
+      <c r="G86">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="H86">
+        <v>1.6</v>
+      </c>
+      <c r="I86">
+        <v>2.11</v>
+      </c>
+      <c r="J86">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87">
         <v>10</v>
       </c>
-      <c r="B84">
+      <c r="B87">
         <v>3.65</v>
       </c>
-      <c r="C84">
+      <c r="C87">
         <v>4.71</v>
       </c>
-      <c r="D84">
+      <c r="D87">
         <v>4.7</v>
       </c>
-      <c r="E84">
+      <c r="E87">
         <v>3.75</v>
       </c>
-      <c r="F84">
+      <c r="F87">
         <v>3.87</v>
       </c>
-      <c r="G84">
+      <c r="G87">
         <v>3.74</v>
       </c>
-      <c r="H84">
+      <c r="H87">
         <v>1.64</v>
       </c>
-      <c r="I84">
+      <c r="I87">
         <v>1.78</v>
       </c>
-      <c r="J84">
+      <c r="J87">
         <v>1.73</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>3</v>
       </c>
-      <c r="B85">
-        <f t="shared" ref="B85:D85" si="23">AVERAGE(B75:B84)</f>
+      <c r="B88">
+        <f t="shared" ref="B88:D88" si="25">AVERAGE(B78:B87)</f>
         <v>3.5569999999999999</v>
       </c>
-      <c r="C85">
-        <f t="shared" si="23"/>
+      <c r="C88">
+        <f t="shared" si="25"/>
         <v>5.346000000000001</v>
       </c>
-      <c r="D85">
-        <f t="shared" si="23"/>
+      <c r="D88">
+        <f t="shared" si="25"/>
         <v>4.7300000000000004</v>
       </c>
-      <c r="E85">
-        <f t="shared" ref="E85:G85" si="24">AVERAGE(E75:E84)</f>
+      <c r="E88">
+        <f t="shared" ref="E88:G88" si="26">AVERAGE(E78:E87)</f>
         <v>3.754</v>
       </c>
-      <c r="F85">
-        <f t="shared" si="24"/>
+      <c r="F88">
+        <f t="shared" si="26"/>
         <v>4.17</v>
       </c>
-      <c r="G85">
-        <f t="shared" si="24"/>
+      <c r="G88">
+        <f t="shared" si="26"/>
         <v>3.8410000000000002</v>
       </c>
-      <c r="H85">
-        <f t="shared" ref="H85:J85" si="25">AVERAGE(H75:H84)</f>
+      <c r="H88">
+        <f t="shared" ref="H88:J88" si="27">AVERAGE(H78:H87)</f>
         <v>1.609</v>
       </c>
-      <c r="I85">
-        <f t="shared" si="25"/>
+      <c r="I88">
+        <f t="shared" si="27"/>
         <v>2.0340000000000003</v>
       </c>
-      <c r="J85">
-        <f t="shared" si="25"/>
+      <c r="J88">
+        <f t="shared" si="27"/>
         <v>1.8030000000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>7</v>
       </c>
-      <c r="B86">
-        <f>STDEV(B75:B84)</f>
+      <c r="B89">
+        <f>STDEV(B78:B87)</f>
         <v>0.11343622780125305</v>
       </c>
-      <c r="C86">
-        <f>STDEV(C75:C84)</f>
+      <c r="C89">
+        <f>STDEV(C78:C87)</f>
         <v>1.6314220109394666</v>
       </c>
-      <c r="D86">
-        <f t="shared" ref="D86" si="26">STDEV(D75:D84)</f>
+      <c r="D89">
+        <f t="shared" ref="D89" si="28">STDEV(D78:D87)</f>
         <v>0.11680943645290154</v>
       </c>
-      <c r="E86">
-        <f t="shared" ref="E86:G86" si="27">STDEV(E75:E84)</f>
+      <c r="E89">
+        <f t="shared" ref="E89:G89" si="29">STDEV(E78:E87)</f>
         <v>6.168017869984193E-2</v>
       </c>
-      <c r="F86">
-        <f t="shared" si="27"/>
+      <c r="F89">
+        <f t="shared" si="29"/>
         <v>0.54733698740152026</v>
       </c>
-      <c r="G86">
-        <f t="shared" si="27"/>
+      <c r="G89">
+        <f t="shared" si="29"/>
         <v>0.25757199640747697</v>
       </c>
-      <c r="H86">
-        <f t="shared" ref="H86:J86" si="28">STDEV(H75:H84)</f>
+      <c r="H89">
+        <f t="shared" ref="H89:J89" si="30">STDEV(H78:H87)</f>
         <v>2.514402955419474E-2</v>
       </c>
-      <c r="I86">
-        <f t="shared" si="28"/>
+      <c r="I89">
+        <f t="shared" si="30"/>
         <v>0.37369625217399083</v>
       </c>
-      <c r="J86">
-        <f t="shared" si="28"/>
+      <c r="J89">
+        <f t="shared" si="30"/>
         <v>0.1058353018189636</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-      <c r="H88" s="4"/>
-      <c r="I88" s="4"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
-      <c r="I89" s="6"/>
-      <c r="J89" s="6"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="3"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="7"/>
-      <c r="G105" s="7"/>
-      <c r="I105" s="6"/>
-      <c r="J105" s="6"/>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="3"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="3"/>
-      <c r="G120" s="3"/>
-      <c r="H120" s="4"/>
-      <c r="I120" s="4"/>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="1"/>
-      <c r="F121" s="7"/>
-      <c r="G121" s="7"/>
-      <c r="I121" s="6"/>
-      <c r="J121" s="6"/>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136" s="3"/>
-      <c r="B136" s="5"/>
-      <c r="C136" s="3"/>
-      <c r="D136" s="3"/>
-      <c r="E136" s="5"/>
-      <c r="F136" s="3"/>
-      <c r="G136" s="3"/>
-      <c r="H136" s="4"/>
-      <c r="I136" s="4"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C137" s="6"/>
-      <c r="D137" s="6"/>
-      <c r="E137" s="1"/>
-      <c r="F137" s="7"/>
-      <c r="G137" s="7"/>
-      <c r="I137" s="6"/>
-      <c r="J137" s="6"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A152" s="3"/>
-      <c r="B152" s="5"/>
-      <c r="C152" s="3"/>
-      <c r="D152" s="3"/>
-      <c r="E152" s="5"/>
-      <c r="F152" s="3"/>
-      <c r="G152" s="3"/>
-      <c r="H152" s="4"/>
-      <c r="I152" s="4"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C153" s="6"/>
-      <c r="D153" s="6"/>
-      <c r="E153" s="1"/>
-      <c r="F153" s="7"/>
-      <c r="G153" s="7"/>
-      <c r="I153" s="6"/>
-      <c r="J153" s="6"/>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="I92" s="8"/>
+      <c r="J92" s="8"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="3"/>
+      <c r="B107" s="5"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="4"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="9"/>
+      <c r="I108" s="8"/>
+      <c r="J108" s="8"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123" s="3"/>
+      <c r="B123" s="5"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="4"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="9"/>
+      <c r="I124" s="8"/>
+      <c r="J124" s="8"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" s="3"/>
+      <c r="B139" s="5"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3"/>
+      <c r="H139" s="4"/>
+      <c r="I139" s="4"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C140" s="8"/>
+      <c r="D140" s="8"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="I140" s="8"/>
+      <c r="J140" s="8"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" s="3"/>
+      <c r="B155" s="5"/>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3"/>
+      <c r="E155" s="5"/>
+      <c r="F155" s="3"/>
+      <c r="G155" s="3"/>
+      <c r="H155" s="4"/>
+      <c r="I155" s="4"/>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
+      <c r="I156" s="8"/>
+      <c r="J156" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="39">
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="F156:G156"/>
+    <mergeCell ref="I156:J156"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="F124:G124"/>
+    <mergeCell ref="I124:J124"/>
+    <mergeCell ref="C140:D140"/>
+    <mergeCell ref="F140:G140"/>
+    <mergeCell ref="I140:J140"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="I108:J108"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="F92:G92"/>
+    <mergeCell ref="I92:J92"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="H6:J6"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="I105:J105"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="F153:G153"/>
-    <mergeCell ref="I153:J153"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="I121:J121"/>
-    <mergeCell ref="C137:D137"/>
-    <mergeCell ref="F137:G137"/>
-    <mergeCell ref="I137:J137"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="I89:J89"/>
-    <mergeCell ref="C105:D105"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5687,47 +5767,47 @@
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="8" t="e">
+      <c r="B5" s="7" t="e">
         <f>(C3-D3)/D3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="e">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="e">
         <f>(F3-G3)/G3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="e">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7" t="e">
         <f>(I3-J3)/J3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="8" t="e">
+      <c r="B6" s="7" t="e">
         <f>(B3-D3)/D3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="e">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="e">
         <f>(E3-G3)/G3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="e">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7" t="e">
         <f>(H3-J3)/J3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
@@ -5758,19 +5838,19 @@
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="I9" s="6" t="s">
+      <c r="G9" s="9"/>
+      <c r="I9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="6"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -5950,19 +6030,19 @@
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="8"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="I25" s="6" t="s">
+      <c r="G25" s="9"/>
+      <c r="I25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J25" s="6"/>
+      <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -6142,19 +6222,19 @@
       <c r="A41" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="6"/>
+      <c r="D41" s="8"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G41" s="7"/>
-      <c r="I41" s="6" t="s">
+      <c r="G41" s="9"/>
+      <c r="I41" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="6"/>
+      <c r="J41" s="8"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
@@ -6334,19 +6414,19 @@
       <c r="A57" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="6"/>
+      <c r="D57" s="8"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="7" t="s">
+      <c r="F57" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="7"/>
-      <c r="I57" s="6" t="s">
+      <c r="G57" s="9"/>
+      <c r="I57" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J57" s="6"/>
+      <c r="J57" s="8"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
@@ -6526,19 +6606,19 @@
       <c r="A73" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D73" s="6"/>
+      <c r="D73" s="8"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="7" t="s">
+      <c r="F73" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G73" s="7"/>
-      <c r="I73" s="6" t="s">
+      <c r="G73" s="9"/>
+      <c r="I73" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J73" s="6"/>
+      <c r="J73" s="8"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
@@ -6713,13 +6793,13 @@
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
-      <c r="I89" s="6"/>
-      <c r="J89" s="6"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
@@ -6733,13 +6813,13 @@
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="7"/>
-      <c r="G105" s="7"/>
-      <c r="I105" s="6"/>
-      <c r="J105" s="6"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="I105" s="8"/>
+      <c r="J105" s="8"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
@@ -6753,13 +6833,13 @@
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="7"/>
-      <c r="G121" s="7"/>
-      <c r="I121" s="6"/>
-      <c r="J121" s="6"/>
+      <c r="F121" s="9"/>
+      <c r="G121" s="9"/>
+      <c r="I121" s="8"/>
+      <c r="J121" s="8"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
@@ -6773,13 +6853,13 @@
       <c r="I136" s="4"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C137" s="6"/>
-      <c r="D137" s="6"/>
+      <c r="C137" s="8"/>
+      <c r="D137" s="8"/>
       <c r="E137" s="1"/>
-      <c r="F137" s="7"/>
-      <c r="G137" s="7"/>
-      <c r="I137" s="6"/>
-      <c r="J137" s="6"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="9"/>
+      <c r="I137" s="8"/>
+      <c r="J137" s="8"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
@@ -6793,52 +6873,52 @@
       <c r="I152" s="4"/>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C153" s="6"/>
-      <c r="D153" s="6"/>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
       <c r="E153" s="1"/>
-      <c r="F153" s="7"/>
-      <c r="G153" s="7"/>
-      <c r="I153" s="6"/>
-      <c r="J153" s="6"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="9"/>
+      <c r="I153" s="8"/>
+      <c r="J153" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="I89:J89"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="I105:J105"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="I121:J121"/>
     <mergeCell ref="C137:D137"/>
     <mergeCell ref="F137:G137"/>
     <mergeCell ref="I137:J137"/>
     <mergeCell ref="C153:D153"/>
     <mergeCell ref="F153:G153"/>
     <mergeCell ref="I153:J153"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="I105:J105"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="I121:J121"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="I89:J89"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Connor: Finished first complete draft of Dissertation.docx
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -180,6 +180,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -187,9 +190,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -224,7 +224,62 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Caching request times</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2901,8 +2956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3047,76 +3102,76 @@
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="8">
         <f>(C3-D3)/D3</f>
         <v>0.29515399526168429</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8">
         <f>(F3-G3)/G3</f>
         <v>0.34481292517006773</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8">
         <f>(I3-J3)/J3</f>
         <v>0.17856401743100242</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="8">
         <f>(B3-D3)/D3</f>
         <v>-0.20353219900926114</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8">
         <f>(E3-G3)/G3</f>
         <v>-7.4936224489794753E-3</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7">
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8">
         <f>(H3-J3)/J3</f>
         <v>-0.16663208134467727</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="8">
         <f>(D3-B3)/B3</f>
         <v>0.25554353704705229</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8">
         <f t="shared" ref="E7" si="2">(G3-E3)/E3</f>
         <v>7.5502008032127324E-3</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8">
         <f t="shared" ref="H7" si="3">(J3-H3)/H3</f>
         <v>0.19995019920318721</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <f>AVERAGE(B5:J5)</f>
         <v>0.27284364595425142</v>
       </c>
@@ -3130,7 +3185,7 @@
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="7">
         <f>AVERAGE(B6:J6)</f>
         <v>-0.12588596760097262</v>
       </c>
@@ -3147,7 +3202,7 @@
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="7">
         <f>AVERAGE(B7:J7)</f>
         <v>0.15434797901781741</v>
       </c>
@@ -3177,19 +3232,19 @@
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="I12" s="8" t="s">
+      <c r="G12" s="10"/>
+      <c r="I12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="8"/>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -3639,19 +3694,19 @@
       <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="8"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="I28" s="8" t="s">
+      <c r="G28" s="10"/>
+      <c r="I28" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J28" s="8"/>
+      <c r="J28" s="9"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -4101,19 +4156,19 @@
       <c r="A44" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="8"/>
+      <c r="D44" s="9"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="I44" s="8" t="s">
+      <c r="G44" s="10"/>
+      <c r="I44" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J44" s="8"/>
+      <c r="J44" s="9"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -4563,19 +4618,19 @@
       <c r="A60" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="8"/>
+      <c r="D60" s="9"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="9" t="s">
+      <c r="F60" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="9"/>
-      <c r="I60" s="8" t="s">
+      <c r="G60" s="10"/>
+      <c r="I60" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J60" s="8"/>
+      <c r="J60" s="9"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
@@ -5025,19 +5080,19 @@
       <c r="A76" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D76" s="8"/>
+      <c r="D76" s="9"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="9" t="s">
+      <c r="F76" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G76" s="9"/>
-      <c r="I76" s="8" t="s">
+      <c r="G76" s="10"/>
+      <c r="I76" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J76" s="8"/>
+      <c r="J76" s="9"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
@@ -5482,13 +5537,13 @@
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
       <c r="E92" s="1"/>
-      <c r="F92" s="9"/>
-      <c r="G92" s="9"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="8"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
+      <c r="I92" s="9"/>
+      <c r="J92" s="9"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
@@ -5502,13 +5557,13 @@
       <c r="I107" s="4"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C108" s="8"/>
-      <c r="D108" s="8"/>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
       <c r="E108" s="1"/>
-      <c r="F108" s="9"/>
-      <c r="G108" s="9"/>
-      <c r="I108" s="8"/>
-      <c r="J108" s="8"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="10"/>
+      <c r="I108" s="9"/>
+      <c r="J108" s="9"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
@@ -5522,13 +5577,13 @@
       <c r="I123" s="4"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C124" s="8"/>
-      <c r="D124" s="8"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="9"/>
-      <c r="G124" s="9"/>
-      <c r="I124" s="8"/>
-      <c r="J124" s="8"/>
+      <c r="F124" s="10"/>
+      <c r="G124" s="10"/>
+      <c r="I124" s="9"/>
+      <c r="J124" s="9"/>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
@@ -5542,13 +5597,13 @@
       <c r="I139" s="4"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C140" s="8"/>
-      <c r="D140" s="8"/>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
       <c r="E140" s="1"/>
-      <c r="F140" s="9"/>
-      <c r="G140" s="9"/>
-      <c r="I140" s="8"/>
-      <c r="J140" s="8"/>
+      <c r="F140" s="10"/>
+      <c r="G140" s="10"/>
+      <c r="I140" s="9"/>
+      <c r="J140" s="9"/>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
@@ -5562,16 +5617,39 @@
       <c r="I155" s="4"/>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C156" s="8"/>
-      <c r="D156" s="8"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
       <c r="E156" s="1"/>
-      <c r="F156" s="9"/>
-      <c r="G156" s="9"/>
-      <c r="I156" s="8"/>
-      <c r="J156" s="8"/>
+      <c r="F156" s="10"/>
+      <c r="G156" s="10"/>
+      <c r="I156" s="9"/>
+      <c r="J156" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="F92:G92"/>
+    <mergeCell ref="I92:J92"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="H7:J7"/>
@@ -5588,29 +5666,6 @@
     <mergeCell ref="I108:J108"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="F60:G60"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="F92:G92"/>
-    <mergeCell ref="I92:J92"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5767,47 +5822,47 @@
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="7" t="e">
+      <c r="B5" s="8" t="e">
         <f>(C3-D3)/D3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="e">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="e">
         <f>(F3-G3)/G3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="e">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="e">
         <f>(I3-J3)/J3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="7" t="e">
+      <c r="B6" s="8" t="e">
         <f>(B3-D3)/D3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="e">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="e">
         <f>(E3-G3)/G3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7" t="e">
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="e">
         <f>(H3-J3)/J3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
@@ -5838,19 +5893,19 @@
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="I9" s="8" t="s">
+      <c r="G9" s="10"/>
+      <c r="I9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="8"/>
+      <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -6030,19 +6085,19 @@
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="I25" s="8" t="s">
+      <c r="G25" s="10"/>
+      <c r="I25" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J25" s="8"/>
+      <c r="J25" s="9"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -6222,19 +6277,19 @@
       <c r="A41" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="8"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G41" s="9"/>
-      <c r="I41" s="8" t="s">
+      <c r="G41" s="10"/>
+      <c r="I41" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="8"/>
+      <c r="J41" s="9"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
@@ -6414,19 +6469,19 @@
       <c r="A57" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="8"/>
+      <c r="D57" s="9"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="9" t="s">
+      <c r="F57" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="9"/>
-      <c r="I57" s="8" t="s">
+      <c r="G57" s="10"/>
+      <c r="I57" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J57" s="8"/>
+      <c r="J57" s="9"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
@@ -6606,19 +6661,19 @@
       <c r="A73" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D73" s="8"/>
+      <c r="D73" s="9"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="9" t="s">
+      <c r="F73" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G73" s="9"/>
-      <c r="I73" s="8" t="s">
+      <c r="G73" s="10"/>
+      <c r="I73" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J73" s="8"/>
+      <c r="J73" s="9"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
@@ -6793,13 +6848,13 @@
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="9"/>
-      <c r="G89" s="9"/>
-      <c r="I89" s="8"/>
-      <c r="J89" s="8"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
@@ -6813,13 +6868,13 @@
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="9"/>
-      <c r="G105" s="9"/>
-      <c r="I105" s="8"/>
-      <c r="J105" s="8"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="9"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
@@ -6833,13 +6888,13 @@
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C121" s="8"/>
-      <c r="D121" s="8"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="9"/>
-      <c r="G121" s="9"/>
-      <c r="I121" s="8"/>
-      <c r="J121" s="8"/>
+      <c r="F121" s="10"/>
+      <c r="G121" s="10"/>
+      <c r="I121" s="9"/>
+      <c r="J121" s="9"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
@@ -6853,13 +6908,13 @@
       <c r="I136" s="4"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C137" s="8"/>
-      <c r="D137" s="8"/>
+      <c r="C137" s="9"/>
+      <c r="D137" s="9"/>
       <c r="E137" s="1"/>
-      <c r="F137" s="9"/>
-      <c r="G137" s="9"/>
-      <c r="I137" s="8"/>
-      <c r="J137" s="8"/>
+      <c r="F137" s="10"/>
+      <c r="G137" s="10"/>
+      <c r="I137" s="9"/>
+      <c r="J137" s="9"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
@@ -6873,52 +6928,52 @@
       <c r="I152" s="4"/>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
       <c r="E153" s="1"/>
-      <c r="F153" s="9"/>
-      <c r="G153" s="9"/>
-      <c r="I153" s="8"/>
-      <c r="J153" s="8"/>
+      <c r="F153" s="10"/>
+      <c r="G153" s="10"/>
+      <c r="I153" s="9"/>
+      <c r="J153" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="F137:G137"/>
+    <mergeCell ref="I137:J137"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="F153:G153"/>
+    <mergeCell ref="I153:J153"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="I105:J105"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="I121:J121"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="I89:J89"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="I25:J25"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="H6:J6"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="I89:J89"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="I105:J105"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="I121:J121"/>
-    <mergeCell ref="C137:D137"/>
-    <mergeCell ref="F137:G137"/>
-    <mergeCell ref="I137:J137"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="F153:G153"/>
-    <mergeCell ref="I153:J153"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Connor: Ran experiment with slower internet.
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Latency Of Requests (Router)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="33">
   <si>
     <t>First Request</t>
   </si>
@@ -162,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -181,6 +181,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -921,7 +924,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6.2303999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -976,7 +979,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.7756000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1013,7 +1016,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7.6245999999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2956,25 +2959,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -2987,7 +2990,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>24</v>
       </c>
@@ -3016,7 +3019,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -3057,7 +3060,7 @@
         <v>1.9276</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3098,76 +3101,76 @@
         <v>0.1173651257542631</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="9">
         <f>(C3-D3)/D3</f>
         <v>0.29515399526168429</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
         <f>(F3-G3)/G3</f>
         <v>0.34481292517006773</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9">
         <f>(I3-J3)/J3</f>
         <v>0.17856401743100242</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="9">
         <f>(B3-D3)/D3</f>
         <v>-0.20353219900926114</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9">
         <f>(E3-G3)/G3</f>
         <v>-7.4936224489794753E-3</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
         <f>(H3-J3)/J3</f>
         <v>-0.16663208134467727</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="9">
         <f>(D3-B3)/B3</f>
         <v>0.25554353704705229</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
         <f t="shared" ref="E7" si="2">(G3-E3)/E3</f>
         <v>7.5502008032127324E-3</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
         <f t="shared" ref="H7" si="3">(J3-H3)/H3</f>
         <v>0.19995019920318721</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
@@ -3181,7 +3184,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -3198,7 +3201,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -3215,7 +3218,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -3228,25 +3231,25 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="9"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="I12" s="9" t="s">
+      <c r="G12" s="11"/>
+      <c r="I12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -3275,7 +3278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3307,7 +3310,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3339,7 +3342,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3371,7 +3374,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
@@ -3403,7 +3406,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>6</v>
       </c>
@@ -3467,7 +3470,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>7</v>
       </c>
@@ -3499,7 +3502,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>8</v>
       </c>
@@ -3531,7 +3534,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>9</v>
       </c>
@@ -3563,7 +3566,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>10</v>
       </c>
@@ -3595,7 +3598,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -3636,7 +3639,7 @@
         <v>1.8700000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -3677,7 +3680,7 @@
         <v>2.1081851067789131E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>9</v>
       </c>
@@ -3690,25 +3693,25 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="9"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="10"/>
-      <c r="I28" s="9" t="s">
+      <c r="G28" s="11"/>
+      <c r="I28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>23</v>
       </c>
@@ -3737,7 +3740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1</v>
       </c>
@@ -3769,7 +3772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2</v>
       </c>
@@ -3801,7 +3804,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3</v>
       </c>
@@ -3833,7 +3836,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3865,7 +3868,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>5</v>
       </c>
@@ -3897,7 +3900,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>6</v>
       </c>
@@ -3929,7 +3932,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>7</v>
       </c>
@@ -3961,7 +3964,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>8</v>
       </c>
@@ -3993,7 +3996,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>9</v>
       </c>
@@ -4025,7 +4028,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>10</v>
       </c>
@@ -4057,7 +4060,7 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -4098,7 +4101,7 @@
         <v>2.1879999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4139,7 +4142,7 @@
         <v>0.11438725647747847</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>10</v>
       </c>
@@ -4152,25 +4155,25 @@
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="9"/>
+      <c r="D44" s="10"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="10"/>
-      <c r="I44" s="9" t="s">
+      <c r="G44" s="11"/>
+      <c r="I44" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J44" s="9"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J44" s="10"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>23</v>
       </c>
@@ -4199,7 +4202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1</v>
       </c>
@@ -4231,7 +4234,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2</v>
       </c>
@@ -4263,7 +4266,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>3</v>
       </c>
@@ -4295,7 +4298,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>4</v>
       </c>
@@ -4327,7 +4330,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>5</v>
       </c>
@@ -4359,7 +4362,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>6</v>
       </c>
@@ -4391,7 +4394,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>7</v>
       </c>
@@ -4423,7 +4426,7 @@
         <v>2.21</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>8</v>
       </c>
@@ -4455,7 +4458,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>9</v>
       </c>
@@ -4487,7 +4490,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>10</v>
       </c>
@@ -4519,7 +4522,7 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -4560,7 +4563,7 @@
         <v>1.921</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -4601,7 +4604,7 @@
         <v>0.23718019403913904</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>13</v>
       </c>
@@ -4614,25 +4617,25 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="9"/>
+      <c r="D60" s="10"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="10" t="s">
+      <c r="F60" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="10"/>
-      <c r="I60" s="9" t="s">
+      <c r="G60" s="11"/>
+      <c r="I60" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J60" s="9"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J60" s="10"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>23</v>
       </c>
@@ -4661,7 +4664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1</v>
       </c>
@@ -4693,7 +4696,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2</v>
       </c>
@@ -4725,7 +4728,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>3</v>
       </c>
@@ -4757,7 +4760,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>4</v>
       </c>
@@ -4789,7 +4792,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>5</v>
       </c>
@@ -4821,7 +4824,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>6</v>
       </c>
@@ -4853,7 +4856,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>7</v>
       </c>
@@ -4885,7 +4888,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>8</v>
       </c>
@@ -4917,7 +4920,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>9</v>
       </c>
@@ -4949,7 +4952,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>10</v>
       </c>
@@ -4981,7 +4984,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -5022,7 +5025,7 @@
         <v>1.8559999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -5063,7 +5066,7 @@
         <v>0.10834102536794532</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>14</v>
       </c>
@@ -5076,25 +5079,25 @@
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C76" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D76" s="9"/>
+      <c r="D76" s="10"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="10" t="s">
+      <c r="F76" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G76" s="10"/>
-      <c r="I76" s="9" t="s">
+      <c r="G76" s="11"/>
+      <c r="I76" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J76" s="9"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J76" s="10"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>23</v>
       </c>
@@ -5123,7 +5126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1</v>
       </c>
@@ -5155,7 +5158,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>2</v>
       </c>
@@ -5187,7 +5190,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>3</v>
       </c>
@@ -5219,7 +5222,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>4</v>
       </c>
@@ -5251,7 +5254,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>5</v>
       </c>
@@ -5283,7 +5286,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>6</v>
       </c>
@@ -5315,7 +5318,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>7</v>
       </c>
@@ -5347,7 +5350,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>8</v>
       </c>
@@ -5379,7 +5382,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>9</v>
       </c>
@@ -5411,7 +5414,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>10</v>
       </c>
@@ -5443,7 +5446,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -5484,7 +5487,7 @@
         <v>1.8030000000000002</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -5525,7 +5528,7 @@
         <v>0.1058353018189636</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="3"/>
       <c r="B91" s="5"/>
       <c r="C91" s="3"/>
@@ -5536,16 +5539,16 @@
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
       <c r="E92" s="1"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="10"/>
-      <c r="I92" s="9"/>
-      <c r="J92" s="9"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="I92" s="10"/>
+      <c r="J92" s="10"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="3"/>
       <c r="B107" s="5"/>
       <c r="C107" s="3"/>
@@ -5556,16 +5559,16 @@
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C108" s="9"/>
-      <c r="D108" s="9"/>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C108" s="10"/>
+      <c r="D108" s="10"/>
       <c r="E108" s="1"/>
-      <c r="F108" s="10"/>
-      <c r="G108" s="10"/>
-      <c r="I108" s="9"/>
-      <c r="J108" s="9"/>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+      <c r="I108" s="10"/>
+      <c r="J108" s="10"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="3"/>
       <c r="B123" s="5"/>
       <c r="C123" s="3"/>
@@ -5576,16 +5579,16 @@
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C124" s="9"/>
-      <c r="D124" s="9"/>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C124" s="10"/>
+      <c r="D124" s="10"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="10"/>
-      <c r="G124" s="10"/>
-      <c r="I124" s="9"/>
-      <c r="J124" s="9"/>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F124" s="11"/>
+      <c r="G124" s="11"/>
+      <c r="I124" s="10"/>
+      <c r="J124" s="10"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="3"/>
       <c r="B139" s="5"/>
       <c r="C139" s="3"/>
@@ -5596,16 +5599,16 @@
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C140" s="9"/>
-      <c r="D140" s="9"/>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C140" s="10"/>
+      <c r="D140" s="10"/>
       <c r="E140" s="1"/>
-      <c r="F140" s="10"/>
-      <c r="G140" s="10"/>
-      <c r="I140" s="9"/>
-      <c r="J140" s="9"/>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F140" s="11"/>
+      <c r="G140" s="11"/>
+      <c r="I140" s="10"/>
+      <c r="J140" s="10"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="3"/>
       <c r="B155" s="5"/>
       <c r="C155" s="3"/>
@@ -5616,23 +5619,34 @@
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C156" s="9"/>
-      <c r="D156" s="9"/>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C156" s="10"/>
+      <c r="D156" s="10"/>
       <c r="E156" s="1"/>
-      <c r="F156" s="10"/>
-      <c r="G156" s="10"/>
-      <c r="I156" s="9"/>
-      <c r="J156" s="9"/>
+      <c r="F156" s="11"/>
+      <c r="G156" s="11"/>
+      <c r="I156" s="10"/>
+      <c r="J156" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="I92:J92"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="F156:G156"/>
+    <mergeCell ref="I156:J156"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="F124:G124"/>
+    <mergeCell ref="I124:J124"/>
+    <mergeCell ref="C140:D140"/>
+    <mergeCell ref="F140:G140"/>
+    <mergeCell ref="I140:J140"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="I108:J108"/>
+    <mergeCell ref="C60:D60"/>
     <mergeCell ref="C108:D108"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="F44:G44"/>
@@ -5649,23 +5663,12 @@
     <mergeCell ref="I76:J76"/>
     <mergeCell ref="C92:D92"/>
     <mergeCell ref="F92:G92"/>
-    <mergeCell ref="I92:J92"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="F156:G156"/>
-    <mergeCell ref="I156:J156"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="F124:G124"/>
-    <mergeCell ref="I124:J124"/>
-    <mergeCell ref="C140:D140"/>
-    <mergeCell ref="F140:G140"/>
-    <mergeCell ref="I140:J140"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="I108:J108"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5676,25 +5679,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="8" max="8" width="20.453125" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -5707,7 +5710,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>24</v>
       </c>
@@ -5736,21 +5739,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="5" t="e">
+      <c r="B3" s="5">
         <f>AVERAGE(B21,B37,B53,B69,B85)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C3" s="5" t="e">
+        <v>6.2303999999999995</v>
+      </c>
+      <c r="C3" s="5">
         <f>AVERAGE(C21,C37,C53,C69,C85)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D3" s="5" t="e">
+        <v>8.7756000000000007</v>
+      </c>
+      <c r="D3" s="5">
         <f t="shared" ref="D3:J4" si="0">AVERAGE(D21,D37,D53,D69,D85)</f>
-        <v>#DIV/0!</v>
+        <v>7.6245999999999992</v>
       </c>
       <c r="E3" s="5" t="e">
         <f>AVERAGE(E21,E37,E53,E69,E85)</f>
@@ -5777,21 +5780,21 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="e">
+      <c r="B4" s="5">
         <f>AVERAGE(B22,B38,B54,B70,B86)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C4" s="5" t="e">
+        <v>1.4207987403312619</v>
+      </c>
+      <c r="C4" s="5">
         <f>AVERAGE(C22,C38,C54,C70,C86)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D4" s="5" t="e">
+        <v>1.7588108743607287</v>
+      </c>
+      <c r="D4" s="5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.1525220801398395</v>
       </c>
       <c r="E4" s="5" t="e">
         <f t="shared" si="0"/>
@@ -5818,57 +5821,62 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="8" t="e">
+      <c r="B5" s="9">
         <f>(C3-D3)/D3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="e">
+        <v>0.15095873881908581</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="e">
         <f>(F3-G3)/G3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="e">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="e">
         <f>(I3-J3)/J3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="8" t="e">
+      <c r="B6" s="9">
         <f>(B3-D3)/D3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="e">
+        <v>-0.18285549405870469</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="e">
         <f>(E3-G3)/G3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="e">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="e">
         <f>(H3-J3)/J3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="9">
+        <f>(D3-B3)/B3</f>
+        <v>0.22377375449409345</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -5876,7 +5884,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -5889,25 +5897,25 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="I9" s="9" t="s">
+      <c r="G9" s="11"/>
+      <c r="I9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -5936,71 +5944,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>4.22</v>
+      </c>
+      <c r="C11">
+        <v>9.09</v>
+      </c>
+      <c r="D11">
+        <v>5.23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>8.81</v>
+      </c>
+      <c r="C12">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="D12">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>6.61</v>
+      </c>
+      <c r="C13">
+        <v>6.54</v>
+      </c>
+      <c r="D13">
+        <v>7.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>6.44</v>
+      </c>
+      <c r="C14">
+        <v>7.35</v>
+      </c>
+      <c r="D14">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>5.77</v>
+      </c>
+      <c r="C15">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="D15">
+        <v>7.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>6.95</v>
+      </c>
+      <c r="C16">
+        <v>5.32</v>
+      </c>
+      <c r="D16">
+        <v>7.37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="C17">
+        <v>9.43</v>
+      </c>
+      <c r="D17">
+        <v>7.82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>6.33</v>
+      </c>
+      <c r="C18">
+        <v>9.49</v>
+      </c>
+      <c r="D18">
+        <v>7.58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>5.69</v>
+      </c>
+      <c r="C19">
+        <v>10.23</v>
+      </c>
+      <c r="D19">
+        <v>7.47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>4.28</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="B21" t="e">
+      <c r="B21">
         <f t="shared" ref="B21:J21" si="1">AVERAGE(B11:B20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" t="e">
+        <v>5.9459999999999997</v>
+      </c>
+      <c r="C21">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D21" t="e">
+        <v>8.2029999999999994</v>
+      </c>
+      <c r="D21">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>6.972999999999999</v>
       </c>
       <c r="E21" t="e">
         <f t="shared" si="1"/>
@@ -6027,21 +6125,21 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B22" t="e">
+      <c r="B22">
         <f>STDEV(B11:B20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C22" t="e">
+        <v>1.4302074441609263</v>
+      </c>
+      <c r="C22">
         <f>STDEV(C11:C20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D22" t="e">
+        <v>1.4919714772370452</v>
+      </c>
+      <c r="D22">
         <f t="shared" ref="D22:J22" si="2">STDEV(D11:D20)</f>
-        <v>#DIV/0!</v>
+        <v>0.94856675510419419</v>
       </c>
       <c r="E22" t="e">
         <f t="shared" si="2"/>
@@ -6068,7 +6166,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
@@ -6081,25 +6179,25 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="9"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="10"/>
-      <c r="I25" s="9" t="s">
+      <c r="G25" s="11"/>
+      <c r="I25" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>23</v>
       </c>
@@ -6128,71 +6226,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>4.21</v>
+      </c>
+      <c r="C27">
+        <v>10.83</v>
+      </c>
+      <c r="D27">
+        <v>9.26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>6.63</v>
+      </c>
+      <c r="C28">
+        <v>7.52</v>
+      </c>
+      <c r="D28">
+        <v>10.98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>5.68</v>
+      </c>
+      <c r="C29">
+        <v>11.66</v>
+      </c>
+      <c r="D29">
+        <v>8.0500000000000007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>6.69</v>
+      </c>
+      <c r="C30">
+        <v>11.04</v>
+      </c>
+      <c r="D30">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>6.76</v>
+      </c>
+      <c r="C31">
+        <v>10.3</v>
+      </c>
+      <c r="D31">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>5.49</v>
+      </c>
+      <c r="C32">
+        <v>16.29</v>
+      </c>
+      <c r="D32">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>5.84</v>
+      </c>
+      <c r="C33">
+        <v>11.75</v>
+      </c>
+      <c r="D33">
+        <v>8.83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>6.74</v>
+      </c>
+      <c r="C34">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D34">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>3.86</v>
+      </c>
+      <c r="C35">
+        <v>6.28</v>
+      </c>
+      <c r="D35">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>6.6</v>
+      </c>
+      <c r="C36">
+        <v>10.64</v>
+      </c>
+      <c r="D36">
+        <v>7.17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>3</v>
       </c>
-      <c r="B37" t="e">
+      <c r="B37">
         <f t="shared" ref="B37:J37" si="3">AVERAGE(B27:B36)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C37" t="e">
+        <v>5.85</v>
+      </c>
+      <c r="C37">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D37" t="e">
+        <v>10.550999999999998</v>
+      </c>
+      <c r="D37">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>7.9380000000000006</v>
       </c>
       <c r="E37" t="e">
         <f t="shared" si="3"/>
@@ -6219,21 +6407,21 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>7</v>
       </c>
-      <c r="B38" t="e">
+      <c r="B38">
         <f>STDEV(B27:B36)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C38" t="e">
+        <v>1.0700467279516321</v>
+      </c>
+      <c r="C38">
         <f>STDEV(C27:C36)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D38" t="e">
+        <v>2.6924810945379787</v>
+      </c>
+      <c r="D38">
         <f t="shared" ref="D38:J38" si="4">STDEV(D27:D36)</f>
-        <v>#DIV/0!</v>
+        <v>1.7763933498336804</v>
       </c>
       <c r="E38" t="e">
         <f t="shared" si="4"/>
@@ -6260,7 +6448,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>10</v>
       </c>
@@ -6273,25 +6461,25 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="9"/>
+      <c r="D41" s="10"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G41" s="10"/>
-      <c r="I41" s="9" t="s">
+      <c r="G41" s="11"/>
+      <c r="I41" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="9"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J41" s="10"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>23</v>
       </c>
@@ -6320,71 +6508,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>6.87</v>
+      </c>
+      <c r="C43">
+        <v>7.13</v>
+      </c>
+      <c r="D43">
+        <v>7.91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>10.31</v>
+      </c>
+      <c r="C44">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="D44">
+        <v>7.67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>5.05</v>
+      </c>
+      <c r="C45">
+        <v>8.18</v>
+      </c>
+      <c r="D45">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>7.23</v>
+      </c>
+      <c r="C46">
+        <v>6.83</v>
+      </c>
+      <c r="D46">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>5.44</v>
+      </c>
+      <c r="C47">
+        <v>8.77</v>
+      </c>
+      <c r="D47">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>9.36</v>
+      </c>
+      <c r="D48">
+        <v>7.82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>4.41</v>
+      </c>
+      <c r="C49">
+        <v>7.69</v>
+      </c>
+      <c r="D49">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>5.07</v>
+      </c>
+      <c r="C50">
+        <v>8.43</v>
+      </c>
+      <c r="D50">
+        <v>5.47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>6.02</v>
+      </c>
+      <c r="C51">
+        <v>6.91</v>
+      </c>
+      <c r="D51">
+        <v>8.69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>4.16</v>
+      </c>
+      <c r="C52">
+        <v>10.32</v>
+      </c>
+      <c r="D52">
+        <v>7.06</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>3</v>
       </c>
-      <c r="B53" t="e">
+      <c r="B53">
         <f t="shared" ref="B53:J53" si="5">AVERAGE(B43:B52)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C53" t="e">
+        <v>6.1560000000000006</v>
+      </c>
+      <c r="C53">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D53" t="e">
+        <v>8.3149999999999977</v>
+      </c>
+      <c r="D53">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>7.2739999999999991</v>
       </c>
       <c r="E53" t="e">
         <f t="shared" si="5"/>
@@ -6411,21 +6689,21 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>7</v>
       </c>
-      <c r="B54" t="e">
+      <c r="B54">
         <f>STDEV(B43:B52)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C54" t="e">
+        <v>1.8134571036191256</v>
+      </c>
+      <c r="C54">
         <f>STDEV(C43:C52)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D54" t="e">
+        <v>1.1926091843796529</v>
+      </c>
+      <c r="D54">
         <f t="shared" ref="D54:J54" si="6">STDEV(D43:D52)</f>
-        <v>#DIV/0!</v>
+        <v>1.1901745903671321</v>
       </c>
       <c r="E54" t="e">
         <f t="shared" si="6"/>
@@ -6452,7 +6730,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>13</v>
       </c>
@@ -6465,25 +6743,25 @@
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="9"/>
+      <c r="D57" s="10"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="10"/>
-      <c r="I57" s="9" t="s">
+      <c r="G57" s="11"/>
+      <c r="I57" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J57" s="9"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J57" s="10"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>23</v>
       </c>
@@ -6512,71 +6790,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>10.33</v>
+      </c>
+      <c r="C59">
+        <v>7.39</v>
+      </c>
+      <c r="D59">
+        <v>8.6199999999999992</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>7.57</v>
+      </c>
+      <c r="C60">
+        <v>6.93</v>
+      </c>
+      <c r="D60">
+        <v>7.96</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>6.15</v>
+      </c>
+      <c r="C61">
+        <v>7.46</v>
+      </c>
+      <c r="D61">
+        <v>8.73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>7.14</v>
+      </c>
+      <c r="D62">
+        <v>8.35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="C63">
+        <v>11.23</v>
+      </c>
+      <c r="D63">
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>6</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>7.33</v>
+      </c>
+      <c r="C64">
+        <v>11.39</v>
+      </c>
+      <c r="D64">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>7</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>5.83</v>
+      </c>
+      <c r="C65">
+        <v>6.39</v>
+      </c>
+      <c r="D65">
+        <v>8.41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>8</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>4.76</v>
+      </c>
+      <c r="C66">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="D66">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>5.2</v>
+      </c>
+      <c r="C67">
+        <v>8.86</v>
+      </c>
+      <c r="D67">
+        <v>8.86</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>6.21</v>
+      </c>
+      <c r="C68">
+        <v>6.67</v>
+      </c>
+      <c r="D68">
+        <v>4.67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>3</v>
       </c>
-      <c r="B69" t="e">
+      <c r="B69">
         <f t="shared" ref="B69:J69" si="7">AVERAGE(B59:B68)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C69" t="e">
+        <v>7.0659999999999981</v>
+      </c>
+      <c r="C69">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D69" t="e">
+        <v>8.293000000000001</v>
+      </c>
+      <c r="D69">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>7.910000000000001</v>
       </c>
       <c r="E69" t="e">
         <f t="shared" si="7"/>
@@ -6603,21 +6971,21 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>7</v>
       </c>
-      <c r="B70" t="e">
+      <c r="B70">
         <f>STDEV(B59:B68)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C70" t="e">
+        <v>1.7842097534887755</v>
+      </c>
+      <c r="C70">
         <f>STDEV(C59:C68)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D70" t="e">
+        <v>1.8522121908679838</v>
+      </c>
+      <c r="D70">
         <f t="shared" ref="D70:J70" si="8">STDEV(D59:D68)</f>
-        <v>#DIV/0!</v>
+        <v>1.4817557153593124</v>
       </c>
       <c r="E70" t="e">
         <f t="shared" si="8"/>
@@ -6644,7 +7012,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>14</v>
       </c>
@@ -6657,25 +7025,25 @@
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D73" s="9"/>
+      <c r="D73" s="10"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="10" t="s">
+      <c r="F73" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G73" s="10"/>
-      <c r="I73" s="9" t="s">
+      <c r="G73" s="11"/>
+      <c r="I73" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J73" s="9"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J73" s="10"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>23</v>
       </c>
@@ -6704,71 +7072,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>5.68</v>
+      </c>
+      <c r="C75">
+        <v>11.59</v>
+      </c>
+      <c r="D75">
+        <v>8.17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>7.7</v>
+      </c>
+      <c r="C76">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="D76">
+        <v>7.83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>3</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>5.07</v>
+      </c>
+      <c r="C77">
+        <v>7.65</v>
+      </c>
+      <c r="D77">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>7.46</v>
+      </c>
+      <c r="C78">
+        <v>8.43</v>
+      </c>
+      <c r="D78">
+        <v>8.7799999999999994</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>4.5</v>
+      </c>
+      <c r="C79">
+        <v>6.41</v>
+      </c>
+      <c r="D79">
+        <v>7.93</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>6.45</v>
+      </c>
+      <c r="C80">
+        <v>7.78</v>
+      </c>
+      <c r="D80">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>7</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>5.7</v>
+      </c>
+      <c r="C81">
+        <v>10.36</v>
+      </c>
+      <c r="D81">
+        <v>7.83</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>8</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>6.81</v>
+      </c>
+      <c r="C82">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="D82">
+        <v>7.59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>6.21</v>
+      </c>
+      <c r="C83">
+        <v>7.15</v>
+      </c>
+      <c r="D83">
+        <v>7.83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>10</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>5.76</v>
+      </c>
+      <c r="C84">
+        <v>7.7</v>
+      </c>
+      <c r="D84">
+        <v>7.79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>3</v>
       </c>
-      <c r="B85" t="e">
+      <c r="B85">
         <f t="shared" ref="B85:J85" si="9">AVERAGE(B75:B84)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C85" t="e">
+        <v>6.1340000000000003</v>
+      </c>
+      <c r="C85">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D85" t="e">
+        <v>8.5160000000000018</v>
+      </c>
+      <c r="D85">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>8.0280000000000005</v>
       </c>
       <c r="E85" t="e">
         <f t="shared" si="9"/>
@@ -6795,21 +7253,21 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>7</v>
       </c>
-      <c r="B86" t="e">
+      <c r="B86">
         <f>STDEV(B75:B84)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C86" t="e">
+        <v>1.0060726724358489</v>
+      </c>
+      <c r="C86">
         <f>STDEV(C75:C84)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D86" t="e">
+        <v>1.564780424780982</v>
+      </c>
+      <c r="D86">
         <f t="shared" ref="D86:J86" si="10">STDEV(D75:D84)</f>
-        <v>#DIV/0!</v>
+        <v>0.3657199900348776</v>
       </c>
       <c r="E86" t="e">
         <f t="shared" si="10"/>
@@ -6836,7 +7294,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -6847,16 +7305,16 @@
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="9"/>
-      <c r="D89" s="9"/>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
-      <c r="I89" s="9"/>
-      <c r="J89" s="9"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="10"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="5"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
@@ -6867,16 +7325,16 @@
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C105" s="9"/>
-      <c r="D105" s="9"/>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="10"/>
-      <c r="G105" s="10"/>
-      <c r="I105" s="9"/>
-      <c r="J105" s="9"/>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F105" s="11"/>
+      <c r="G105" s="11"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="10"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="5"/>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
@@ -6887,16 +7345,16 @@
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C121" s="9"/>
-      <c r="D121" s="9"/>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="10"/>
-      <c r="G121" s="10"/>
-      <c r="I121" s="9"/>
-      <c r="J121" s="9"/>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F121" s="11"/>
+      <c r="G121" s="11"/>
+      <c r="I121" s="10"/>
+      <c r="J121" s="10"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="5"/>
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
@@ -6907,16 +7365,16 @@
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C137" s="9"/>
-      <c r="D137" s="9"/>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
       <c r="E137" s="1"/>
-      <c r="F137" s="10"/>
-      <c r="G137" s="10"/>
-      <c r="I137" s="9"/>
-      <c r="J137" s="9"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F137" s="11"/>
+      <c r="G137" s="11"/>
+      <c r="I137" s="10"/>
+      <c r="J137" s="10"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="5"/>
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
@@ -6927,53 +7385,54 @@
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C153" s="9"/>
-      <c r="D153" s="9"/>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
       <c r="E153" s="1"/>
-      <c r="F153" s="10"/>
-      <c r="G153" s="10"/>
-      <c r="I153" s="9"/>
-      <c r="J153" s="9"/>
+      <c r="F153" s="11"/>
+      <c r="G153" s="11"/>
+      <c r="I153" s="10"/>
+      <c r="J153" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="37">
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="I89:J89"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="I105:J105"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="I121:J121"/>
     <mergeCell ref="C137:D137"/>
     <mergeCell ref="F137:G137"/>
     <mergeCell ref="I137:J137"/>
     <mergeCell ref="C153:D153"/>
     <mergeCell ref="F153:G153"/>
     <mergeCell ref="I153:J153"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="I105:J105"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="I121:J121"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="I89:J89"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Connor: Tidied Dissertation.docx up to implementation. Added new experimental results for caching.
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12650" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Latency Of Requests (Router)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="34">
   <si>
     <t>First Request</t>
   </si>
@@ -120,6 +120,9 @@
   <si>
     <t>% Diff on cached</t>
   </si>
+  <si>
+    <t xml:space="preserve"> BBC (3G)</t>
+  </si>
 </sst>
 </file>
 
@@ -186,13 +189,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1488,6 +1491,432 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Caching request times (3G network)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>BBC No Cache</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Mobile)'!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6.2303999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-65E2-4D56-A75B-42F42907F574}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>BBC Not Cached</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-65E2-4D56-A75B-42F42907F574}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Mobile)'!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8.7756000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-65E2-4D56-A75B-42F42907F574}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BBC Cached</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Mobile)'!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.6245999999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-65E2-4D56-A75B-42F42907F574}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1520754464"/>
+        <c:axId val="1617533696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1520754464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1617533696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1617533696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Request</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1520754464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1568,6 +1997,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2072,6 +2541,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2652,6 +3624,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BA045C2-79A5-4836-BECC-2DC093307501}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2960,24 +3970,24 @@
   <dimension ref="A1:J156"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:D7"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -2990,7 +4000,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>24</v>
       </c>
@@ -3019,7 +4029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -3060,7 +4070,7 @@
         <v>1.9276</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3101,76 +4111,76 @@
         <v>0.1173651257542631</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="11">
         <f>(C3-D3)/D3</f>
         <v>0.29515399526168429</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11">
         <f>(F3-G3)/G3</f>
         <v>0.34481292517006773</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11">
         <f>(I3-J3)/J3</f>
         <v>0.17856401743100242</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="11">
         <f>(B3-D3)/D3</f>
         <v>-0.20353219900926114</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11">
         <f>(E3-G3)/G3</f>
         <v>-7.4936224489794753E-3</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11">
         <f>(H3-J3)/J3</f>
         <v>-0.16663208134467727</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="11">
         <f>(D3-B3)/B3</f>
         <v>0.25554353704705229</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11">
         <f t="shared" ref="E7" si="2">(G3-E3)/E3</f>
         <v>7.5502008032127324E-3</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11">
         <f t="shared" ref="H7" si="3">(J3-H3)/H3</f>
         <v>0.19995019920318721</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
@@ -3184,7 +4194,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -3201,7 +4211,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -3218,7 +4228,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -3231,7 +4241,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -3240,16 +4250,16 @@
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="9"/>
       <c r="I12" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -3278,7 +4288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3310,7 +4320,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3342,7 +4352,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3374,7 +4384,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -3406,7 +4416,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -3438,7 +4448,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -3470,7 +4480,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -3502,7 +4512,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
@@ -3534,7 +4544,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -3566,7 +4576,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
@@ -3598,7 +4608,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -3639,7 +4649,7 @@
         <v>1.8700000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -3680,7 +4690,7 @@
         <v>2.1081851067789131E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>9</v>
       </c>
@@ -3693,7 +4703,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -3702,16 +4712,16 @@
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="11"/>
+      <c r="G28" s="9"/>
       <c r="I28" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>23</v>
       </c>
@@ -3740,7 +4750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -3772,7 +4782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -3804,7 +4814,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -3836,7 +4846,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3868,7 +4878,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5</v>
       </c>
@@ -3900,7 +4910,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6</v>
       </c>
@@ -3932,7 +4942,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
@@ -3964,7 +4974,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8</v>
       </c>
@@ -3996,7 +5006,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9</v>
       </c>
@@ -4028,7 +5038,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10</v>
       </c>
@@ -4060,7 +5070,7 @@
         <v>2.13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -4101,7 +5111,7 @@
         <v>2.1879999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4142,7 +5152,7 @@
         <v>0.11438725647747847</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>10</v>
       </c>
@@ -4155,7 +5165,7 @@
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -4164,16 +5174,16 @@
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="11"/>
+      <c r="G44" s="9"/>
       <c r="I44" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>23</v>
       </c>
@@ -4202,7 +5212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -4234,7 +5244,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2</v>
       </c>
@@ -4266,7 +5276,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -4298,7 +5308,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
@@ -4330,7 +5340,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5</v>
       </c>
@@ -4362,7 +5372,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6</v>
       </c>
@@ -4394,7 +5404,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7</v>
       </c>
@@ -4426,7 +5436,7 @@
         <v>2.21</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>8</v>
       </c>
@@ -4458,7 +5468,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9</v>
       </c>
@@ -4490,7 +5500,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>10</v>
       </c>
@@ -4522,7 +5532,7 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -4563,7 +5573,7 @@
         <v>1.921</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -4604,7 +5614,7 @@
         <v>0.23718019403913904</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>13</v>
       </c>
@@ -4617,7 +5627,7 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -4626,16 +5636,16 @@
       </c>
       <c r="D60" s="10"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="11" t="s">
+      <c r="F60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="11"/>
+      <c r="G60" s="9"/>
       <c r="I60" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J60" s="10"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>23</v>
       </c>
@@ -4664,7 +5674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1</v>
       </c>
@@ -4696,7 +5706,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
@@ -4728,7 +5738,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3</v>
       </c>
@@ -4760,7 +5770,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>4</v>
       </c>
@@ -4792,7 +5802,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5</v>
       </c>
@@ -4824,7 +5834,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>6</v>
       </c>
@@ -4856,7 +5866,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>7</v>
       </c>
@@ -4888,7 +5898,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>8</v>
       </c>
@@ -4920,7 +5930,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9</v>
       </c>
@@ -4952,7 +5962,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>10</v>
       </c>
@@ -4984,7 +5994,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -5025,7 +6035,7 @@
         <v>1.8559999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -5066,7 +6076,7 @@
         <v>0.10834102536794532</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>14</v>
       </c>
@@ -5079,7 +6089,7 @@
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -5088,16 +6098,16 @@
       </c>
       <c r="D76" s="10"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="11" t="s">
+      <c r="F76" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G76" s="11"/>
+      <c r="G76" s="9"/>
       <c r="I76" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J76" s="10"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>23</v>
       </c>
@@ -5126,7 +6136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1</v>
       </c>
@@ -5158,7 +6168,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2</v>
       </c>
@@ -5190,7 +6200,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>3</v>
       </c>
@@ -5222,7 +6232,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>4</v>
       </c>
@@ -5254,7 +6264,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>5</v>
       </c>
@@ -5286,7 +6296,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>6</v>
       </c>
@@ -5318,7 +6328,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>7</v>
       </c>
@@ -5350,7 +6360,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>8</v>
       </c>
@@ -5382,7 +6392,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>9</v>
       </c>
@@ -5414,7 +6424,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>10</v>
       </c>
@@ -5446,7 +6456,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -5487,7 +6497,7 @@
         <v>1.8030000000000002</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -5528,7 +6538,7 @@
         <v>0.1058353018189636</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="5"/>
       <c r="C91" s="3"/>
@@ -5539,16 +6549,16 @@
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C92" s="10"/>
       <c r="D92" s="10"/>
       <c r="E92" s="1"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="11"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
       <c r="I92" s="10"/>
       <c r="J92" s="10"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="5"/>
       <c r="C107" s="3"/>
@@ -5559,16 +6569,16 @@
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C108" s="10"/>
       <c r="D108" s="10"/>
       <c r="E108" s="1"/>
-      <c r="F108" s="11"/>
-      <c r="G108" s="11"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="9"/>
       <c r="I108" s="10"/>
       <c r="J108" s="10"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="5"/>
       <c r="C123" s="3"/>
@@ -5579,16 +6589,16 @@
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C124" s="10"/>
       <c r="D124" s="10"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="11"/>
-      <c r="G124" s="11"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="9"/>
       <c r="I124" s="10"/>
       <c r="J124" s="10"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="5"/>
       <c r="C139" s="3"/>
@@ -5599,16 +6609,16 @@
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C140" s="10"/>
       <c r="D140" s="10"/>
       <c r="E140" s="1"/>
-      <c r="F140" s="11"/>
-      <c r="G140" s="11"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
       <c r="I140" s="10"/>
       <c r="J140" s="10"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="5"/>
       <c r="C155" s="3"/>
@@ -5619,22 +6629,36 @@
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C156" s="10"/>
       <c r="D156" s="10"/>
       <c r="E156" s="1"/>
-      <c r="F156" s="11"/>
-      <c r="G156" s="11"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
       <c r="I156" s="10"/>
       <c r="J156" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="I92:J92"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="I108:J108"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="F92:G92"/>
     <mergeCell ref="C156:D156"/>
     <mergeCell ref="F156:G156"/>
     <mergeCell ref="I156:J156"/>
@@ -5644,31 +6668,17 @@
     <mergeCell ref="C140:D140"/>
     <mergeCell ref="F140:G140"/>
     <mergeCell ref="I140:J140"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="I108:J108"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="I92:J92"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="F92:G92"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5680,24 +6690,24 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
-    <col min="8" max="8" width="20.453125" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -5710,7 +6720,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>24</v>
       </c>
@@ -5739,7 +6749,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -5780,7 +6790,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -5821,62 +6831,62 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="11">
         <f>(C3-D3)/D3</f>
         <v>0.15095873881908581</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9" t="e">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="e">
         <f>(F3-G3)/G3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9" t="e">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="e">
         <f>(I3-J3)/J3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="11">
         <f>(B3-D3)/D3</f>
         <v>-0.18285549405870469</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="e">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="e">
         <f>(E3-G3)/G3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9" t="e">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11" t="e">
         <f>(H3-J3)/J3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="11">
         <f>(D3-B3)/B3</f>
         <v>0.22377375449409345</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -5884,7 +6894,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -5897,25 +6907,25 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="11"/>
+      <c r="G9" s="9"/>
       <c r="I9" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -5944,7 +6954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -5958,7 +6968,7 @@
         <v>5.23</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -5972,7 +6982,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -5986,7 +6996,7 @@
         <v>7.41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -6000,7 +7010,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -6014,7 +7024,7 @@
         <v>7.41</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -6028,7 +7038,7 @@
         <v>7.37</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -6042,7 +7052,7 @@
         <v>7.82</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
@@ -6056,7 +7066,7 @@
         <v>7.58</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -6070,7 +7080,7 @@
         <v>7.47</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -6084,7 +7094,7 @@
         <v>6.64</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -6125,7 +7135,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -6166,7 +7176,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
@@ -6179,25 +7189,25 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="11"/>
+      <c r="G25" s="9"/>
       <c r="I25" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>23</v>
       </c>
@@ -6226,7 +7236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -6240,7 +7250,7 @@
         <v>9.26</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -6254,7 +7264,7 @@
         <v>10.98</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -6268,7 +7278,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
@@ -6282,7 +7292,7 @@
         <v>5.81</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -6296,7 +7306,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -6310,7 +7320,7 @@
         <v>8.99</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -6324,7 +7334,7 @@
         <v>8.83</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8</v>
       </c>
@@ -6338,7 +7348,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9</v>
       </c>
@@ -6352,7 +7362,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10</v>
       </c>
@@ -6366,7 +7376,7 @@
         <v>7.17</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -6407,7 +7417,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -6448,7 +7458,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>10</v>
       </c>
@@ -6461,25 +7471,25 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>2</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G41" s="11"/>
+      <c r="G41" s="9"/>
       <c r="I41" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>23</v>
       </c>
@@ -6508,7 +7518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -6522,7 +7532,7 @@
         <v>7.91</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -6536,7 +7546,7 @@
         <v>7.67</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -6550,7 +7560,7 @@
         <v>7.71</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -6564,7 +7574,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5</v>
       </c>
@@ -6578,7 +7588,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>6</v>
       </c>
@@ -6592,7 +7602,7 @@
         <v>7.82</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7</v>
       </c>
@@ -6606,7 +7616,7 @@
         <v>5.68</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>8</v>
       </c>
@@ -6620,7 +7630,7 @@
         <v>5.47</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>9</v>
       </c>
@@ -6634,7 +7644,7 @@
         <v>8.69</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>10</v>
       </c>
@@ -6648,7 +7658,7 @@
         <v>7.06</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -6689,7 +7699,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -6730,7 +7740,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>13</v>
       </c>
@@ -6743,25 +7753,25 @@
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>2</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="11" t="s">
+      <c r="F57" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="11"/>
+      <c r="G57" s="9"/>
       <c r="I57" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J57" s="10"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>23</v>
       </c>
@@ -6790,7 +7800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -6804,7 +7814,7 @@
         <v>8.6199999999999992</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2</v>
       </c>
@@ -6818,7 +7828,7 @@
         <v>7.96</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3</v>
       </c>
@@ -6832,7 +7842,7 @@
         <v>8.73</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4</v>
       </c>
@@ -6846,7 +7856,7 @@
         <v>8.35</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5</v>
       </c>
@@ -6860,7 +7870,7 @@
         <v>9.09</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>6</v>
       </c>
@@ -6874,7 +7884,7 @@
         <v>8.68</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>7</v>
       </c>
@@ -6888,7 +7898,7 @@
         <v>8.41</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>8</v>
       </c>
@@ -6902,7 +7912,7 @@
         <v>5.73</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9</v>
       </c>
@@ -6916,7 +7926,7 @@
         <v>8.86</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>10</v>
       </c>
@@ -6930,7 +7940,7 @@
         <v>4.67</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -6971,7 +7981,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -7012,7 +8022,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>14</v>
       </c>
@@ -7025,25 +8035,25 @@
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>2</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D73" s="10"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="11" t="s">
+      <c r="F73" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G73" s="11"/>
+      <c r="G73" s="9"/>
       <c r="I73" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J73" s="10"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>23</v>
       </c>
@@ -7072,7 +8082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1</v>
       </c>
@@ -7086,7 +8096,7 @@
         <v>8.17</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2</v>
       </c>
@@ -7100,7 +8110,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3</v>
       </c>
@@ -7114,7 +8124,7 @@
         <v>8.52</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4</v>
       </c>
@@ -7128,7 +8138,7 @@
         <v>8.7799999999999994</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5</v>
       </c>
@@ -7142,7 +8152,7 @@
         <v>7.93</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>6</v>
       </c>
@@ -7156,7 +8166,7 @@
         <v>8.01</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>7</v>
       </c>
@@ -7170,7 +8180,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>8</v>
       </c>
@@ -7184,7 +8194,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>9</v>
       </c>
@@ -7198,7 +8208,7 @@
         <v>7.83</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>10</v>
       </c>
@@ -7212,7 +8222,7 @@
         <v>7.79</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>3</v>
       </c>
@@ -7253,7 +8263,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -7294,7 +8304,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -7305,16 +8315,16 @@
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C89" s="10"/>
       <c r="D89" s="10"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
       <c r="I89" s="10"/>
       <c r="J89" s="10"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
@@ -7325,16 +8335,16 @@
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C105" s="10"/>
       <c r="D105" s="10"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="11"/>
-      <c r="G105" s="11"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
       <c r="I105" s="10"/>
       <c r="J105" s="10"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
@@ -7345,16 +8355,16 @@
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C121" s="10"/>
       <c r="D121" s="10"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="11"/>
-      <c r="G121" s="11"/>
+      <c r="F121" s="9"/>
+      <c r="G121" s="9"/>
       <c r="I121" s="10"/>
       <c r="J121" s="10"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
@@ -7365,16 +8375,16 @@
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C137" s="10"/>
       <c r="D137" s="10"/>
       <c r="E137" s="1"/>
-      <c r="F137" s="11"/>
-      <c r="G137" s="11"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="9"/>
       <c r="I137" s="10"/>
       <c r="J137" s="10"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
@@ -7385,17 +8395,47 @@
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C153" s="10"/>
       <c r="D153" s="10"/>
       <c r="E153" s="1"/>
-      <c r="F153" s="11"/>
-      <c r="G153" s="11"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="9"/>
       <c r="I153" s="10"/>
       <c r="J153" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="F137:G137"/>
+    <mergeCell ref="I137:J137"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="F153:G153"/>
+    <mergeCell ref="I153:J153"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="I105:J105"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="I121:J121"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="I89:J89"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="I25:J25"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
@@ -7403,36 +8443,6 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="H6:J6"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="I89:J89"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="I105:J105"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="I121:J121"/>
-    <mergeCell ref="C137:D137"/>
-    <mergeCell ref="F137:G137"/>
-    <mergeCell ref="I137:J137"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="F153:G153"/>
-    <mergeCell ref="I153:J153"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Connor: Updated experimentation section (apart from Machine Learning) developed upon evaluation of the machine learning application in order to provide some numbers.
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Latency Of Requests (Router)" sheetId="1" r:id="rId1"/>
@@ -189,14 +189,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -296,7 +296,7 @@
           <c:idx val="6"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>BBC No Cache</c:v>
+            <c:v>BBC without using a cache</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -332,7 +332,7 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>BBC Not Cached</c:v>
+            <c:v>BBC without a populated cache</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -387,7 +387,7 @@
           <c:idx val="1"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>BBC Cached</c:v>
+            <c:v>BBC with a populated cache</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -424,7 +424,7 @@
           <c:idx val="7"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Sky News No Cache</c:v>
+            <c:v>Sky News without using a cache</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -460,7 +460,7 @@
           <c:idx val="2"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>Sky News Not Cached</c:v>
+            <c:v>Sky News without a populated cache</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -496,7 +496,7 @@
           <c:idx val="3"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>Sky News Cached</c:v>
+            <c:v>Sky News with a populated cache</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -533,7 +533,7 @@
           <c:idx val="8"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>A Single Div No Cache</c:v>
+            <c:v>A Single Div without using a cache</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -569,7 +569,7 @@
           <c:idx val="4"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>A Single Div Not Cached</c:v>
+            <c:v>A Single Div without a populated cache</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -626,7 +626,7 @@
           <c:idx val="5"/>
           <c:order val="8"/>
           <c:tx>
-            <c:v>A Single Div Cached</c:v>
+            <c:v>A Single Div with a populated cache</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -3551,13 +3551,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>182218</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>67918</xdr:rowOff>
     </xdr:to>
@@ -3969,8 +3969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4115,70 +4115,70 @@
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <f>(C3-D3)/D3</f>
         <v>0.29515399526168429</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
         <f>(F3-G3)/G3</f>
         <v>0.34481292517006773</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9">
         <f>(I3-J3)/J3</f>
         <v>0.17856401743100242</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <f>(B3-D3)/D3</f>
         <v>-0.20353219900926114</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9">
         <f>(E3-G3)/G3</f>
         <v>-7.4936224489794753E-3</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
         <f>(H3-J3)/J3</f>
         <v>-0.16663208134467727</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <f>(D3-B3)/B3</f>
         <v>0.25554353704705229</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
         <f t="shared" ref="E7" si="2">(G3-E3)/E3</f>
         <v>7.5502008032127324E-3</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
         <f t="shared" ref="H7" si="3">(J3-H3)/H3</f>
         <v>0.19995019920318721</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -4245,19 +4245,19 @@
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="I12" s="10" t="s">
+      <c r="G12" s="10"/>
+      <c r="I12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="10"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -4707,19 +4707,19 @@
       <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="11"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="I28" s="10" t="s">
+      <c r="G28" s="10"/>
+      <c r="I28" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J28" s="10"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -5169,19 +5169,19 @@
       <c r="A44" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="10"/>
+      <c r="D44" s="11"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="I44" s="10" t="s">
+      <c r="G44" s="10"/>
+      <c r="I44" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J44" s="10"/>
+      <c r="J44" s="11"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -5631,19 +5631,19 @@
       <c r="A60" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="10"/>
+      <c r="D60" s="11"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="9" t="s">
+      <c r="F60" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="9"/>
-      <c r="I60" s="10" t="s">
+      <c r="G60" s="10"/>
+      <c r="I60" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J60" s="10"/>
+      <c r="J60" s="11"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
@@ -6093,19 +6093,19 @@
       <c r="A76" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C76" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D76" s="10"/>
+      <c r="D76" s="11"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="9" t="s">
+      <c r="F76" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G76" s="9"/>
-      <c r="I76" s="10" t="s">
+      <c r="G76" s="10"/>
+      <c r="I76" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J76" s="10"/>
+      <c r="J76" s="11"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
@@ -6550,13 +6550,13 @@
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
       <c r="E92" s="1"/>
-      <c r="F92" s="9"/>
-      <c r="G92" s="9"/>
-      <c r="I92" s="10"/>
-      <c r="J92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
@@ -6570,13 +6570,13 @@
       <c r="I107" s="4"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
       <c r="E108" s="1"/>
-      <c r="F108" s="9"/>
-      <c r="G108" s="9"/>
-      <c r="I108" s="10"/>
-      <c r="J108" s="10"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="10"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="11"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
@@ -6590,13 +6590,13 @@
       <c r="I123" s="4"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
+      <c r="C124" s="11"/>
+      <c r="D124" s="11"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="9"/>
-      <c r="G124" s="9"/>
-      <c r="I124" s="10"/>
-      <c r="J124" s="10"/>
+      <c r="F124" s="10"/>
+      <c r="G124" s="10"/>
+      <c r="I124" s="11"/>
+      <c r="J124" s="11"/>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
@@ -6610,13 +6610,13 @@
       <c r="I139" s="4"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C140" s="10"/>
-      <c r="D140" s="10"/>
+      <c r="C140" s="11"/>
+      <c r="D140" s="11"/>
       <c r="E140" s="1"/>
-      <c r="F140" s="9"/>
-      <c r="G140" s="9"/>
-      <c r="I140" s="10"/>
-      <c r="J140" s="10"/>
+      <c r="F140" s="10"/>
+      <c r="G140" s="10"/>
+      <c r="I140" s="11"/>
+      <c r="J140" s="11"/>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
@@ -6630,22 +6630,34 @@
       <c r="I155" s="4"/>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C156" s="10"/>
-      <c r="D156" s="10"/>
+      <c r="C156" s="11"/>
+      <c r="D156" s="11"/>
       <c r="E156" s="1"/>
-      <c r="F156" s="9"/>
-      <c r="G156" s="9"/>
-      <c r="I156" s="10"/>
-      <c r="J156" s="10"/>
+      <c r="F156" s="10"/>
+      <c r="G156" s="10"/>
+      <c r="I156" s="11"/>
+      <c r="J156" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="F156:G156"/>
+    <mergeCell ref="I156:J156"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="F124:G124"/>
+    <mergeCell ref="I124:J124"/>
+    <mergeCell ref="C140:D140"/>
+    <mergeCell ref="F140:G140"/>
+    <mergeCell ref="I140:J140"/>
     <mergeCell ref="F108:G108"/>
     <mergeCell ref="I108:J108"/>
     <mergeCell ref="C60:D60"/>
@@ -6659,26 +6671,14 @@
     <mergeCell ref="I76:J76"/>
     <mergeCell ref="C92:D92"/>
     <mergeCell ref="F92:G92"/>
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="F156:G156"/>
-    <mergeCell ref="I156:J156"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="F124:G124"/>
-    <mergeCell ref="I124:J124"/>
-    <mergeCell ref="C140:D140"/>
-    <mergeCell ref="F140:G140"/>
-    <mergeCell ref="I140:J140"/>
     <mergeCell ref="F60:G60"/>
     <mergeCell ref="I92:J92"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6689,7 +6689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
@@ -6835,58 +6835,58 @@
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <f>(C3-D3)/D3</f>
         <v>0.15095873881908581</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="e">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="e">
         <f>(F3-G3)/G3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11" t="e">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="e">
         <f>(I3-J3)/J3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <f>(B3-D3)/D3</f>
         <v>-0.18285549405870469</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="e">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="e">
         <f>(E3-G3)/G3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11" t="e">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="e">
         <f>(H3-J3)/J3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <f>(D3-B3)/B3</f>
         <v>0.22377375449409345</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -6911,19 +6911,19 @@
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="I9" s="10" t="s">
+      <c r="G9" s="10"/>
+      <c r="I9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -7193,19 +7193,19 @@
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="I25" s="10" t="s">
+      <c r="G25" s="10"/>
+      <c r="I25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J25" s="10"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -7475,19 +7475,19 @@
       <c r="A41" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="10"/>
+      <c r="D41" s="11"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G41" s="9"/>
-      <c r="I41" s="10" t="s">
+      <c r="G41" s="10"/>
+      <c r="I41" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="10"/>
+      <c r="J41" s="11"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
@@ -7757,19 +7757,19 @@
       <c r="A57" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="10"/>
+      <c r="D57" s="11"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="9" t="s">
+      <c r="F57" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="9"/>
-      <c r="I57" s="10" t="s">
+      <c r="G57" s="10"/>
+      <c r="I57" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J57" s="10"/>
+      <c r="J57" s="11"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
@@ -8039,19 +8039,19 @@
       <c r="A73" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D73" s="10"/>
+      <c r="D73" s="11"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="9" t="s">
+      <c r="F73" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G73" s="9"/>
-      <c r="I73" s="10" t="s">
+      <c r="G73" s="10"/>
+      <c r="I73" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J73" s="10"/>
+      <c r="J73" s="11"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
@@ -8316,13 +8316,13 @@
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="9"/>
-      <c r="G89" s="9"/>
-      <c r="I89" s="10"/>
-      <c r="J89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="11"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
@@ -8336,13 +8336,13 @@
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="9"/>
-      <c r="G105" s="9"/>
-      <c r="I105" s="10"/>
-      <c r="J105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="I105" s="11"/>
+      <c r="J105" s="11"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
@@ -8356,13 +8356,13 @@
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="9"/>
-      <c r="G121" s="9"/>
-      <c r="I121" s="10"/>
-      <c r="J121" s="10"/>
+      <c r="F121" s="10"/>
+      <c r="G121" s="10"/>
+      <c r="I121" s="11"/>
+      <c r="J121" s="11"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
@@ -8376,13 +8376,13 @@
       <c r="I136" s="4"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C137" s="10"/>
-      <c r="D137" s="10"/>
+      <c r="C137" s="11"/>
+      <c r="D137" s="11"/>
       <c r="E137" s="1"/>
-      <c r="F137" s="9"/>
-      <c r="G137" s="9"/>
-      <c r="I137" s="10"/>
-      <c r="J137" s="10"/>
+      <c r="F137" s="10"/>
+      <c r="G137" s="10"/>
+      <c r="I137" s="11"/>
+      <c r="J137" s="11"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
@@ -8396,46 +8396,16 @@
       <c r="I152" s="4"/>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C153" s="10"/>
-      <c r="D153" s="10"/>
+      <c r="C153" s="11"/>
+      <c r="D153" s="11"/>
       <c r="E153" s="1"/>
-      <c r="F153" s="9"/>
-      <c r="G153" s="9"/>
-      <c r="I153" s="10"/>
-      <c r="J153" s="10"/>
+      <c r="F153" s="10"/>
+      <c r="G153" s="10"/>
+      <c r="I153" s="11"/>
+      <c r="J153" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C137:D137"/>
-    <mergeCell ref="F137:G137"/>
-    <mergeCell ref="I137:J137"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="F153:G153"/>
-    <mergeCell ref="I153:J153"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="I105:J105"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="I121:J121"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="I89:J89"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="I25:J25"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
@@ -8443,6 +8413,36 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="H6:J6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="I89:J89"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="I105:J105"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="I121:J121"/>
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="F137:G137"/>
+    <mergeCell ref="I137:J137"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="F153:G153"/>
+    <mergeCell ref="I153:J153"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Connor: Fixed bug in caching client application. Performed experimentation with a more powerful edge node which involved adapting code to ensure it worked on windows.
</commit_message>
<xml_diff>
--- a/Documentation/Experiments/CachingApplication.xlsx
+++ b/Documentation/Experiments/CachingApplication.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12645" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Latency Of Requests (Router)" sheetId="1" r:id="rId1"/>
     <sheet name="Latency Of Requests (Mobile)" sheetId="3" r:id="rId2"/>
+    <sheet name="Latency Of Requests (Windows)" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="40">
   <si>
     <t>First Request</t>
   </si>
@@ -123,13 +124,46 @@
   <si>
     <t xml:space="preserve"> BBC (3G)</t>
   </si>
+  <si>
+    <t xml:space="preserve"> BBC - using 1 data centre redis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BBC - without Electron</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BBC - using 3 edge redis instances</t>
+  </si>
+  <si>
+    <t>REDOING THE BBC ONE!</t>
+  </si>
+  <si>
+    <t>BBC - Again</t>
+  </si>
+  <si>
+    <t>COPIED</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -165,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -197,6 +231,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1917,6 +1974,1033 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>BBC No Cache</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.9560000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-72A9-4975-B39A-9D5865FF1562}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>BBC Not Cached</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-72A9-4975-B39A-9D5865FF1562}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.5944000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-72A9-4975-B39A-9D5865FF1562}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BBC Cached</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.3212000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-72A9-4975-B39A-9D5865FF1562}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Sky News No Cache</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.9560000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-72A9-4975-B39A-9D5865FF1562}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Sky News Not Cached</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.5347999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-72A9-4975-B39A-9D5865FF1562}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Sky News Cached</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.1467999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-72A9-4975-B39A-9D5865FF1562}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>A Single Div No Cache</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-72A9-4975-B39A-9D5865FF1562}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>A Single Div Not Cached</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-72A9-4975-B39A-9D5865FF1562}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-72A9-4975-B39A-9D5865FF1562}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>A Single Div Cached</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-72A9-4975-B39A-9D5865FF1562}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1520754464"/>
+        <c:axId val="1617533696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1520754464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1617533696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1617533696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Request</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1520754464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Caching request times (Windows)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.9560000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9110-4385-AF9F-37C2F02ED8DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-9110-4385-AF9F-37C2F02ED8DB}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.5944000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9110-4385-AF9F-37C2F02ED8DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Latency Of Requests (Windows)'!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.3212000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-9110-4385-AF9F-37C2F02ED8DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1520754464"/>
+        <c:axId val="1617533696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1520754464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1617533696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1617533696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Request</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1520754464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2037,6 +3121,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3044,6 +4208,1012 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3648,6 +5818,87 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BA045C2-79A5-4836-BECC-2DC093307501}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>182218</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>67918</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0E45DED-D071-4C7D-BA8E-4B86D4F15886}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBCFB4DC-5E11-4471-9850-4258D1CD88F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3969,7 +6220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
@@ -6689,8 +8940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6714,9 +8965,11 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="E1" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
@@ -6730,15 +8983,9 @@
       <c r="D2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="5" t="s">
         <v>26</v>
       </c>
@@ -6915,9 +9162,9 @@
         <v>33</v>
       </c>
       <c r="D9" s="11"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="10" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="G9" s="10"/>
       <c r="I9" s="11" t="s">
@@ -7199,7 +9446,7 @@
       <c r="D25" s="11"/>
       <c r="E25" s="1"/>
       <c r="F25" s="10" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="G25" s="10"/>
       <c r="I25" s="11" t="s">
@@ -7481,7 +9728,7 @@
       <c r="D41" s="11"/>
       <c r="E41" s="1"/>
       <c r="F41" s="10" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="G41" s="10"/>
       <c r="I41" s="11" t="s">
@@ -7763,7 +10010,7 @@
       <c r="D57" s="11"/>
       <c r="E57" s="1"/>
       <c r="F57" s="10" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="G57" s="10"/>
       <c r="I57" s="11" t="s">
@@ -8045,7 +10292,7 @@
       <c r="D73" s="11"/>
       <c r="E73" s="1"/>
       <c r="F73" s="10" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="G73" s="10"/>
       <c r="I73" s="11" t="s">
@@ -8405,7 +10652,8 @@
       <c r="J153" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="38">
+    <mergeCell ref="E1:G2"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
@@ -8445,6 +10693,2213 @@
     <mergeCell ref="I153:J153"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J153"/>
+  <sheetViews>
+    <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" style="14" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="14" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="14" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="12">
+        <f>AVERAGE(B21,B37,B53,B69,B85)</f>
+        <v>3.9560000000000004</v>
+      </c>
+      <c r="C3" s="12">
+        <f>AVERAGE(C21,C37,C53,C69,C85)</f>
+        <v>4.5944000000000003</v>
+      </c>
+      <c r="D3" s="12">
+        <f t="shared" ref="D3:J4" si="0">AVERAGE(D21,D37,D53,D69,D85)</f>
+        <v>4.3212000000000002</v>
+      </c>
+      <c r="E3" s="12">
+        <f>AVERAGE(E21,E37,E53,E69,E85)</f>
+        <v>3.9560000000000004</v>
+      </c>
+      <c r="F3" s="12">
+        <f t="shared" si="0"/>
+        <v>4.5347999999999997</v>
+      </c>
+      <c r="G3" s="12">
+        <f t="shared" si="0"/>
+        <v>4.1467999999999998</v>
+      </c>
+      <c r="H3" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="12">
+        <f>AVERAGE(B22,B38,B54,B70,B86)</f>
+        <v>0.21166750312566038</v>
+      </c>
+      <c r="C4" s="12">
+        <f>AVERAGE(C22,C38,C54,C70,C86)</f>
+        <v>0.21596847817161208</v>
+      </c>
+      <c r="D4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.28172890453894961</v>
+      </c>
+      <c r="E4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.21166750312566038</v>
+      </c>
+      <c r="F4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.2963516671450791</v>
+      </c>
+      <c r="G4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.40030531613981546</v>
+      </c>
+      <c r="H4" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I4" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="15">
+        <f>(C3-D3)/D3</f>
+        <v>6.3223178746644473E-2</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15">
+        <f>(F3-G3)/G3</f>
+        <v>9.3566123275778901E-2</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15" t="e">
+        <f>(I3-J3)/J3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="15">
+        <f>(B3-D3)/D3</f>
+        <v>-8.4513561047857011E-2</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15">
+        <f>(E3-G3)/G3</f>
+        <v>-4.6011382270666396E-2</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="e">
+        <f>(H3-J3)/J3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="15">
+        <f>(D3-B3)/B3</f>
+        <v>9.2315470171890721E-2</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15">
+        <f>(G3-E3)/E3</f>
+        <v>4.8230535894843121E-2</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="e">
+        <f t="shared" ref="H7" si="1">(J3-H3)/H3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="I9" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>1</v>
+      </c>
+      <c r="B11" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="C11" s="14">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="D11" s="14">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="E11" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="F11" s="14">
+        <v>4.78</v>
+      </c>
+      <c r="G11" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>2</v>
+      </c>
+      <c r="B12" s="14">
+        <v>4.05</v>
+      </c>
+      <c r="C12" s="14">
+        <v>4.49</v>
+      </c>
+      <c r="D12" s="14">
+        <v>4.38</v>
+      </c>
+      <c r="E12" s="14">
+        <v>4.05</v>
+      </c>
+      <c r="F12" s="14">
+        <v>4.87</v>
+      </c>
+      <c r="G12" s="14">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>3</v>
+      </c>
+      <c r="B13" s="14">
+        <v>4.17</v>
+      </c>
+      <c r="C13" s="14">
+        <v>4.76</v>
+      </c>
+      <c r="D13" s="14">
+        <v>4.54</v>
+      </c>
+      <c r="E13" s="14">
+        <v>4.17</v>
+      </c>
+      <c r="F13" s="14">
+        <v>4.58</v>
+      </c>
+      <c r="G13" s="14">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>4</v>
+      </c>
+      <c r="B14" s="14">
+        <v>4.13</v>
+      </c>
+      <c r="C14" s="14">
+        <v>4.95</v>
+      </c>
+      <c r="D14" s="14">
+        <v>4.72</v>
+      </c>
+      <c r="E14" s="14">
+        <v>4.13</v>
+      </c>
+      <c r="F14" s="14">
+        <v>4.66</v>
+      </c>
+      <c r="G14" s="14">
+        <v>3.62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>5</v>
+      </c>
+      <c r="B15" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="C15" s="14">
+        <v>4.76</v>
+      </c>
+      <c r="D15" s="14">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="E15" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="F15" s="14">
+        <v>4.59</v>
+      </c>
+      <c r="G15" s="14">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>6</v>
+      </c>
+      <c r="B16" s="14">
+        <v>3.96</v>
+      </c>
+      <c r="C16" s="14">
+        <v>5.17</v>
+      </c>
+      <c r="D16" s="14">
+        <v>3.88</v>
+      </c>
+      <c r="E16" s="14">
+        <v>3.96</v>
+      </c>
+      <c r="F16" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="G16" s="14">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>7</v>
+      </c>
+      <c r="B17" s="14">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="C17" s="14">
+        <v>4.84</v>
+      </c>
+      <c r="D17" s="14">
+        <v>4.04</v>
+      </c>
+      <c r="E17" s="14">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="F17" s="14">
+        <v>3.98</v>
+      </c>
+      <c r="G17" s="14">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>8</v>
+      </c>
+      <c r="B18" s="14">
+        <v>3.59</v>
+      </c>
+      <c r="C18" s="14">
+        <v>4.41</v>
+      </c>
+      <c r="D18" s="14">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="E18" s="14">
+        <v>3.59</v>
+      </c>
+      <c r="F18" s="14">
+        <v>4.66</v>
+      </c>
+      <c r="G18" s="14">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>9</v>
+      </c>
+      <c r="B19" s="14">
+        <v>4</v>
+      </c>
+      <c r="C19" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="D19" s="14">
+        <v>4.45</v>
+      </c>
+      <c r="E19" s="14">
+        <v>4</v>
+      </c>
+      <c r="F19" s="14">
+        <v>3.82</v>
+      </c>
+      <c r="G19" s="14">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>10</v>
+      </c>
+      <c r="B20" s="14">
+        <v>3.87</v>
+      </c>
+      <c r="C20" s="14">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="D20" s="14">
+        <v>4.12</v>
+      </c>
+      <c r="E20" s="14">
+        <v>3.87</v>
+      </c>
+      <c r="F20" s="14">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="G20" s="14">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="14">
+        <f t="shared" ref="B21:J21" si="2">AVERAGE(B11:B20)</f>
+        <v>3.9749999999999992</v>
+      </c>
+      <c r="C21" s="14">
+        <f t="shared" si="2"/>
+        <v>4.75</v>
+      </c>
+      <c r="D21" s="14">
+        <f t="shared" si="2"/>
+        <v>4.3449999999999998</v>
+      </c>
+      <c r="E21" s="14">
+        <f t="shared" si="2"/>
+        <v>3.9749999999999992</v>
+      </c>
+      <c r="F21" s="14">
+        <f t="shared" si="2"/>
+        <v>4.5129999999999999</v>
+      </c>
+      <c r="G21" s="14">
+        <f t="shared" si="2"/>
+        <v>4.0919999999999996</v>
+      </c>
+      <c r="H21" s="14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" s="14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" s="14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="14">
+        <f>STDEV(B11:B20)</f>
+        <v>0.16419838949000412</v>
+      </c>
+      <c r="C22" s="14">
+        <f>STDEV(C11:C20)</f>
+        <v>0.21949436844205761</v>
+      </c>
+      <c r="D22" s="14">
+        <f t="shared" ref="D22:J22" si="3">STDEV(D11:D20)</f>
+        <v>0.26575887149402516</v>
+      </c>
+      <c r="E22" s="14">
+        <f t="shared" si="3"/>
+        <v>0.16419838949000412</v>
+      </c>
+      <c r="F22" s="14">
+        <f t="shared" si="3"/>
+        <v>0.34127375782174912</v>
+      </c>
+      <c r="G22" s="14">
+        <f t="shared" si="3"/>
+        <v>0.32296542642621473</v>
+      </c>
+      <c r="H22" s="14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" s="14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="I25" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>1</v>
+      </c>
+      <c r="B27" s="14">
+        <v>4.12</v>
+      </c>
+      <c r="C27" s="14">
+        <v>4.82</v>
+      </c>
+      <c r="D27" s="14">
+        <v>3.95</v>
+      </c>
+      <c r="E27" s="14">
+        <v>4.12</v>
+      </c>
+      <c r="F27" s="14">
+        <v>5.01</v>
+      </c>
+      <c r="G27" s="14">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>2</v>
+      </c>
+      <c r="B28" s="14">
+        <v>4.13</v>
+      </c>
+      <c r="C28" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="D28" s="14">
+        <v>4.34</v>
+      </c>
+      <c r="E28" s="14">
+        <v>4.13</v>
+      </c>
+      <c r="F28" s="14">
+        <v>4.75</v>
+      </c>
+      <c r="G28" s="14">
+        <v>4.37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>3</v>
+      </c>
+      <c r="B29" s="14">
+        <v>3.87</v>
+      </c>
+      <c r="C29" s="14">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="D29" s="14">
+        <v>4.26</v>
+      </c>
+      <c r="E29" s="14">
+        <v>3.87</v>
+      </c>
+      <c r="F29" s="14">
+        <v>4.74</v>
+      </c>
+      <c r="G29" s="14">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>4</v>
+      </c>
+      <c r="B30" s="14">
+        <v>4.58</v>
+      </c>
+      <c r="C30" s="14">
+        <v>4.16</v>
+      </c>
+      <c r="D30" s="14">
+        <v>4.37</v>
+      </c>
+      <c r="E30" s="14">
+        <v>4.58</v>
+      </c>
+      <c r="F30" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G30" s="14">
+        <v>4.3899999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>5</v>
+      </c>
+      <c r="B31" s="14">
+        <v>3.98</v>
+      </c>
+      <c r="C31" s="14">
+        <v>3.99</v>
+      </c>
+      <c r="D31" s="14">
+        <v>4.18</v>
+      </c>
+      <c r="E31" s="14">
+        <v>3.98</v>
+      </c>
+      <c r="F31" s="14">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="G31" s="14">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>6</v>
+      </c>
+      <c r="B32" s="14">
+        <v>3.78</v>
+      </c>
+      <c r="C32" s="14">
+        <v>5.04</v>
+      </c>
+      <c r="D32" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="E32" s="14">
+        <v>3.78</v>
+      </c>
+      <c r="F32" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="G32" s="14">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>7</v>
+      </c>
+      <c r="B33" s="14">
+        <v>3.58</v>
+      </c>
+      <c r="C33" s="14">
+        <v>3.96</v>
+      </c>
+      <c r="D33" s="14">
+        <v>4.53</v>
+      </c>
+      <c r="E33" s="14">
+        <v>3.58</v>
+      </c>
+      <c r="F33" s="14">
+        <v>4.75</v>
+      </c>
+      <c r="G33" s="14">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>8</v>
+      </c>
+      <c r="B34" s="14">
+        <v>4.07</v>
+      </c>
+      <c r="C34" s="14">
+        <v>4.57</v>
+      </c>
+      <c r="D34" s="14">
+        <v>3.89</v>
+      </c>
+      <c r="E34" s="14">
+        <v>4.07</v>
+      </c>
+      <c r="F34" s="14">
+        <v>3.92</v>
+      </c>
+      <c r="G34" s="14">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>9</v>
+      </c>
+      <c r="B35" s="14">
+        <v>3.66</v>
+      </c>
+      <c r="C35" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="D35" s="14">
+        <v>4.42</v>
+      </c>
+      <c r="E35" s="14">
+        <v>3.66</v>
+      </c>
+      <c r="F35" s="14">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="G35" s="14">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>10</v>
+      </c>
+      <c r="B36" s="14">
+        <v>4.12</v>
+      </c>
+      <c r="C36" s="14">
+        <v>4.45</v>
+      </c>
+      <c r="D36" s="14">
+        <v>4.29</v>
+      </c>
+      <c r="E36" s="14">
+        <v>4.12</v>
+      </c>
+      <c r="F36" s="14">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="G36" s="14">
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="14">
+        <f t="shared" ref="B37:J37" si="4">AVERAGE(B27:B36)</f>
+        <v>3.9890000000000008</v>
+      </c>
+      <c r="C37" s="14">
+        <f t="shared" si="4"/>
+        <v>4.4430000000000005</v>
+      </c>
+      <c r="D37" s="14">
+        <f t="shared" si="4"/>
+        <v>4.2129999999999992</v>
+      </c>
+      <c r="E37" s="14">
+        <f t="shared" si="4"/>
+        <v>3.9890000000000008</v>
+      </c>
+      <c r="F37" s="14">
+        <f t="shared" si="4"/>
+        <v>4.5490000000000004</v>
+      </c>
+      <c r="G37" s="14">
+        <f t="shared" si="4"/>
+        <v>4.1339999999999995</v>
+      </c>
+      <c r="H37" s="14" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I37" s="14" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J37" s="14" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="14">
+        <f>STDEV(B27:B36)</f>
+        <v>0.28741955396249574</v>
+      </c>
+      <c r="C38" s="14">
+        <f>STDEV(C27:C36)</f>
+        <v>0.33990358109976487</v>
+      </c>
+      <c r="D38" s="14">
+        <f t="shared" ref="D38:J38" si="5">STDEV(D27:D36)</f>
+        <v>0.22725658528534559</v>
+      </c>
+      <c r="E38" s="14">
+        <f t="shared" si="5"/>
+        <v>0.28741955396249574</v>
+      </c>
+      <c r="F38" s="14">
+        <f t="shared" si="5"/>
+        <v>0.35120269550977734</v>
+      </c>
+      <c r="G38" s="14">
+        <f t="shared" si="5"/>
+        <v>0.29368161142449634</v>
+      </c>
+      <c r="H38" s="14" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" s="14" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J38" s="14" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="16"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="16"/>
+      <c r="I41" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J41" s="16"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
+        <v>1</v>
+      </c>
+      <c r="B43" s="14">
+        <v>4.16</v>
+      </c>
+      <c r="C43" s="14">
+        <v>4.49</v>
+      </c>
+      <c r="D43" s="14">
+        <v>4.59</v>
+      </c>
+      <c r="E43" s="14">
+        <v>4.16</v>
+      </c>
+      <c r="F43" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="G43" s="14">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
+        <v>2</v>
+      </c>
+      <c r="B44" s="14">
+        <v>4</v>
+      </c>
+      <c r="C44" s="14">
+        <v>4.47</v>
+      </c>
+      <c r="D44" s="14">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="E44" s="14">
+        <v>4</v>
+      </c>
+      <c r="F44" s="14">
+        <v>4.92</v>
+      </c>
+      <c r="G44" s="14">
+        <v>4.04</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>3</v>
+      </c>
+      <c r="B45" s="14">
+        <v>3.99</v>
+      </c>
+      <c r="C45" s="14">
+        <v>4.82</v>
+      </c>
+      <c r="D45" s="14">
+        <v>3.98</v>
+      </c>
+      <c r="E45" s="14">
+        <v>3.99</v>
+      </c>
+      <c r="F45" s="14">
+        <v>4.75</v>
+      </c>
+      <c r="G45" s="14">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
+        <v>4</v>
+      </c>
+      <c r="B46" s="14">
+        <v>3.74</v>
+      </c>
+      <c r="C46" s="14">
+        <v>4.46</v>
+      </c>
+      <c r="D46" s="14">
+        <v>3.64</v>
+      </c>
+      <c r="E46" s="14">
+        <v>3.74</v>
+      </c>
+      <c r="F46" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G46" s="14">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>5</v>
+      </c>
+      <c r="B47" s="14">
+        <v>3.99</v>
+      </c>
+      <c r="C47" s="14">
+        <v>4.62</v>
+      </c>
+      <c r="D47" s="14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E47" s="14">
+        <v>3.99</v>
+      </c>
+      <c r="F47" s="14">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="G47" s="14">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="14">
+        <v>6</v>
+      </c>
+      <c r="B48" s="14">
+        <v>3.39</v>
+      </c>
+      <c r="C48" s="14">
+        <v>4.75</v>
+      </c>
+      <c r="D48" s="14">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="E48" s="14">
+        <v>3.39</v>
+      </c>
+      <c r="F48" s="14">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="G48" s="14">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
+        <v>7</v>
+      </c>
+      <c r="B49" s="14">
+        <v>3.77</v>
+      </c>
+      <c r="C49" s="14">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="D49" s="14">
+        <v>4.24</v>
+      </c>
+      <c r="E49" s="14">
+        <v>3.77</v>
+      </c>
+      <c r="F49" s="14">
+        <v>3.74</v>
+      </c>
+      <c r="G49" s="14">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
+        <v>8</v>
+      </c>
+      <c r="B50" s="14">
+        <v>3.84</v>
+      </c>
+      <c r="C50" s="14">
+        <v>4.78</v>
+      </c>
+      <c r="D50" s="14">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="E50" s="14">
+        <v>3.84</v>
+      </c>
+      <c r="F50" s="14">
+        <v>4.34</v>
+      </c>
+      <c r="G50" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="14">
+        <v>9</v>
+      </c>
+      <c r="B51" s="14">
+        <v>3.74</v>
+      </c>
+      <c r="C51" s="14">
+        <v>4.43</v>
+      </c>
+      <c r="D51" s="14">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="E51" s="14">
+        <v>3.74</v>
+      </c>
+      <c r="F51" s="14">
+        <v>4.7</v>
+      </c>
+      <c r="G51" s="14">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="14">
+        <v>10</v>
+      </c>
+      <c r="B52" s="14">
+        <v>4.04</v>
+      </c>
+      <c r="C52" s="14">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D52" s="14">
+        <v>4.88</v>
+      </c>
+      <c r="E52" s="14">
+        <v>4.04</v>
+      </c>
+      <c r="F52" s="14">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="G52" s="14">
+        <v>4.6500000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="14">
+        <f t="shared" ref="B53:J53" si="6">AVERAGE(B43:B52)</f>
+        <v>3.8660000000000005</v>
+      </c>
+      <c r="C53" s="14">
+        <f t="shared" si="6"/>
+        <v>4.6029999999999998</v>
+      </c>
+      <c r="D53" s="14">
+        <f t="shared" si="6"/>
+        <v>4.3980000000000015</v>
+      </c>
+      <c r="E53" s="14">
+        <f t="shared" si="6"/>
+        <v>3.8660000000000005</v>
+      </c>
+      <c r="F53" s="14">
+        <f t="shared" si="6"/>
+        <v>4.548</v>
+      </c>
+      <c r="G53" s="14">
+        <f t="shared" si="6"/>
+        <v>4.177999999999999</v>
+      </c>
+      <c r="H53" s="14" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I53" s="14" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J53" s="14" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="14">
+        <f>STDEV(B43:B52)</f>
+        <v>0.21950449248756213</v>
+      </c>
+      <c r="C54" s="14">
+        <f>STDEV(C43:C52)</f>
+        <v>0.1434534380518255</v>
+      </c>
+      <c r="D54" s="14">
+        <f t="shared" ref="D54:J54" si="7">STDEV(D43:D52)</f>
+        <v>0.35946874381200061</v>
+      </c>
+      <c r="E54" s="14">
+        <f t="shared" si="7"/>
+        <v>0.21950449248756213</v>
+      </c>
+      <c r="F54" s="14">
+        <f t="shared" si="7"/>
+        <v>0.33352661063249506</v>
+      </c>
+      <c r="G54" s="14">
+        <f t="shared" si="7"/>
+        <v>0.69569789100985713</v>
+      </c>
+      <c r="H54" s="14" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I54" s="14" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J54" s="14" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+    </row>
+    <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" s="16"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G57" s="16"/>
+      <c r="I57" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J57" s="16"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H58" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I58" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J58" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="14">
+        <v>1</v>
+      </c>
+      <c r="B59" s="14">
+        <v>4.25</v>
+      </c>
+      <c r="C59" s="14">
+        <v>4.59</v>
+      </c>
+      <c r="D59" s="14">
+        <v>4</v>
+      </c>
+      <c r="E59" s="14">
+        <v>4.25</v>
+      </c>
+      <c r="F59" s="14">
+        <v>3.98</v>
+      </c>
+      <c r="G59" s="14">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="14">
+        <v>2</v>
+      </c>
+      <c r="B60" s="14">
+        <v>4.03</v>
+      </c>
+      <c r="C60" s="14">
+        <v>4.25</v>
+      </c>
+      <c r="D60" s="14">
+        <v>4.55</v>
+      </c>
+      <c r="E60" s="14">
+        <v>4.03</v>
+      </c>
+      <c r="F60" s="14">
+        <v>4.82</v>
+      </c>
+      <c r="G60" s="14">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="14">
+        <v>3</v>
+      </c>
+      <c r="B61" s="14">
+        <v>3.94</v>
+      </c>
+      <c r="C61" s="14">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="D61" s="14">
+        <v>4.47</v>
+      </c>
+      <c r="E61" s="14">
+        <v>3.94</v>
+      </c>
+      <c r="F61" s="14">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="G61" s="14">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="14">
+        <v>4</v>
+      </c>
+      <c r="B62" s="14">
+        <v>4.24</v>
+      </c>
+      <c r="C62" s="14">
+        <v>4.58</v>
+      </c>
+      <c r="D62" s="14">
+        <v>4.2</v>
+      </c>
+      <c r="E62" s="14">
+        <v>4.24</v>
+      </c>
+      <c r="F62" s="14">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="G62" s="14">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="14">
+        <v>5</v>
+      </c>
+      <c r="B63" s="14">
+        <v>3.99</v>
+      </c>
+      <c r="C63" s="14">
+        <v>4.51</v>
+      </c>
+      <c r="D63" s="14">
+        <v>3.67</v>
+      </c>
+      <c r="E63" s="14">
+        <v>3.99</v>
+      </c>
+      <c r="F63" s="14">
+        <v>4.28</v>
+      </c>
+      <c r="G63" s="14">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="14">
+        <v>6</v>
+      </c>
+      <c r="B64" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C64" s="14">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="D64" s="14">
+        <v>4.5</v>
+      </c>
+      <c r="E64" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F64" s="14">
+        <v>4.82</v>
+      </c>
+      <c r="G64" s="14">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="14">
+        <v>7</v>
+      </c>
+      <c r="B65" s="14">
+        <v>4.32</v>
+      </c>
+      <c r="C65" s="14">
+        <v>4.43</v>
+      </c>
+      <c r="D65" s="14">
+        <v>4.49</v>
+      </c>
+      <c r="E65" s="14">
+        <v>4.32</v>
+      </c>
+      <c r="F65" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G65" s="14">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="14">
+        <v>8</v>
+      </c>
+      <c r="B66" s="14">
+        <v>3.82</v>
+      </c>
+      <c r="C66" s="14">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D66" s="14">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="E66" s="14">
+        <v>3.82</v>
+      </c>
+      <c r="F66" s="14">
+        <v>4.55</v>
+      </c>
+      <c r="G66" s="14">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
+        <v>9</v>
+      </c>
+      <c r="B67" s="14">
+        <v>3.88</v>
+      </c>
+      <c r="C67" s="14">
+        <v>4.74</v>
+      </c>
+      <c r="D67" s="14">
+        <v>4.28</v>
+      </c>
+      <c r="E67" s="14">
+        <v>3.88</v>
+      </c>
+      <c r="F67" s="14">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="G67" s="14">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="14">
+        <v>10</v>
+      </c>
+      <c r="B68" s="14">
+        <v>4.13</v>
+      </c>
+      <c r="C68" s="14">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="D68" s="14">
+        <v>4.42</v>
+      </c>
+      <c r="E68" s="14">
+        <v>4.13</v>
+      </c>
+      <c r="F68" s="14">
+        <v>4.24</v>
+      </c>
+      <c r="G68" s="14">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="14">
+        <f t="shared" ref="B69:J69" si="8">AVERAGE(B59:B68)</f>
+        <v>4.0700000000000012</v>
+      </c>
+      <c r="C69" s="14">
+        <f t="shared" si="8"/>
+        <v>4.5439999999999996</v>
+      </c>
+      <c r="D69" s="14">
+        <f t="shared" si="8"/>
+        <v>4.3020000000000005</v>
+      </c>
+      <c r="E69" s="14">
+        <f t="shared" si="8"/>
+        <v>4.0700000000000012</v>
+      </c>
+      <c r="F69" s="14">
+        <f t="shared" si="8"/>
+        <v>4.4359999999999999</v>
+      </c>
+      <c r="G69" s="14">
+        <f t="shared" si="8"/>
+        <v>4.2100000000000009</v>
+      </c>
+      <c r="H69" s="14" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I69" s="14" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J69" s="14" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="14">
+        <f>STDEV(B59:B68)</f>
+        <v>0.16726559053725845</v>
+      </c>
+      <c r="C70" s="14">
+        <f>STDEV(C59:C68)</f>
+        <v>0.16534139765278935</v>
+      </c>
+      <c r="D70" s="14">
+        <f t="shared" ref="D70:J70" si="9">STDEV(D59:D68)</f>
+        <v>0.27863955210988983</v>
+      </c>
+      <c r="E70" s="14">
+        <f t="shared" si="9"/>
+        <v>0.16726559053725845</v>
+      </c>
+      <c r="F70" s="14">
+        <f t="shared" si="9"/>
+        <v>0.29315145876795123</v>
+      </c>
+      <c r="G70" s="14">
+        <f t="shared" si="9"/>
+        <v>0.32052041016654975</v>
+      </c>
+      <c r="H70" s="14" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I70" s="14" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J70" s="14" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+    </row>
+    <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D73" s="16"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G73" s="16"/>
+      <c r="I73" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J73" s="16"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B74" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F74" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G74" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H74" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I74" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J74" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="14">
+        <v>1</v>
+      </c>
+      <c r="B75" s="14">
+        <v>3.69</v>
+      </c>
+      <c r="C75" s="14">
+        <v>4.78</v>
+      </c>
+      <c r="D75" s="14">
+        <v>4.16</v>
+      </c>
+      <c r="E75" s="14">
+        <v>3.69</v>
+      </c>
+      <c r="F75" s="14">
+        <v>4.46</v>
+      </c>
+      <c r="G75" s="14">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="14">
+        <v>2</v>
+      </c>
+      <c r="B76" s="14">
+        <v>3.81</v>
+      </c>
+      <c r="C76" s="14">
+        <v>4.43</v>
+      </c>
+      <c r="D76" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="E76" s="14">
+        <v>3.81</v>
+      </c>
+      <c r="F76" s="14">
+        <v>4.25</v>
+      </c>
+      <c r="G76" s="14">
+        <v>3.91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="14">
+        <v>3</v>
+      </c>
+      <c r="B77" s="14">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="C77" s="14">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="D77" s="14">
+        <v>4.12</v>
+      </c>
+      <c r="E77" s="14">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="F77" s="14">
+        <v>4.75</v>
+      </c>
+      <c r="G77" s="14">
+        <v>4.3099999999999996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="14">
+        <v>4</v>
+      </c>
+      <c r="B78" s="14">
+        <v>4.03</v>
+      </c>
+      <c r="C78" s="14">
+        <v>4.76</v>
+      </c>
+      <c r="D78" s="14">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="E78" s="14">
+        <v>4.03</v>
+      </c>
+      <c r="F78" s="14">
+        <v>4.8</v>
+      </c>
+      <c r="G78" s="14">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="14">
+        <v>5</v>
+      </c>
+      <c r="B79" s="14">
+        <v>3.72</v>
+      </c>
+      <c r="C79" s="14">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="D79" s="14">
+        <v>4.03</v>
+      </c>
+      <c r="E79" s="14">
+        <v>3.72</v>
+      </c>
+      <c r="F79" s="14">
+        <v>4.72</v>
+      </c>
+      <c r="G79" s="14">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="14">
+        <v>6</v>
+      </c>
+      <c r="B80" s="14">
+        <v>3.74</v>
+      </c>
+      <c r="C80" s="14">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D80" s="14">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="E80" s="14">
+        <v>3.74</v>
+      </c>
+      <c r="F80" s="14">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="G80" s="14">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="14">
+        <v>7</v>
+      </c>
+      <c r="B81" s="14">
+        <v>3.61</v>
+      </c>
+      <c r="C81" s="14">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D81" s="14">
+        <v>4.51</v>
+      </c>
+      <c r="E81" s="14">
+        <v>3.61</v>
+      </c>
+      <c r="F81" s="14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G81" s="14">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="14">
+        <v>8</v>
+      </c>
+      <c r="B82" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="C82" s="14">
+        <v>4.37</v>
+      </c>
+      <c r="D82" s="14">
+        <v>4.57</v>
+      </c>
+      <c r="E82" s="14">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="F82" s="14">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="G82" s="14">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="14">
+        <v>9</v>
+      </c>
+      <c r="B83" s="14">
+        <v>3.75</v>
+      </c>
+      <c r="C83" s="14">
+        <v>4.25</v>
+      </c>
+      <c r="D83" s="14">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="E83" s="14">
+        <v>3.75</v>
+      </c>
+      <c r="F83" s="14">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="G83" s="14">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="14">
+        <v>10</v>
+      </c>
+      <c r="B84" s="14">
+        <v>4.25</v>
+      </c>
+      <c r="C84" s="14">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="D84" s="14">
+        <v>4.51</v>
+      </c>
+      <c r="E84" s="14">
+        <v>4.25</v>
+      </c>
+      <c r="F84" s="14">
+        <v>4.67</v>
+      </c>
+      <c r="G84" s="14">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" s="14">
+        <f t="shared" ref="B85:J85" si="10">AVERAGE(B75:B84)</f>
+        <v>3.88</v>
+      </c>
+      <c r="C85" s="14">
+        <f t="shared" si="10"/>
+        <v>4.6319999999999997</v>
+      </c>
+      <c r="D85" s="14">
+        <f t="shared" si="10"/>
+        <v>4.3479999999999999</v>
+      </c>
+      <c r="E85" s="14">
+        <f t="shared" si="10"/>
+        <v>3.88</v>
+      </c>
+      <c r="F85" s="14">
+        <f t="shared" si="10"/>
+        <v>4.6280000000000001</v>
+      </c>
+      <c r="G85" s="14">
+        <f t="shared" si="10"/>
+        <v>4.12</v>
+      </c>
+      <c r="H85" s="14" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I85" s="14" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J85" s="14" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86" s="14">
+        <f>STDEV(B75:B84)</f>
+        <v>0.21994948915098153</v>
+      </c>
+      <c r="C86" s="14">
+        <f>STDEV(C75:C84)</f>
+        <v>0.21164960561162302</v>
+      </c>
+      <c r="D86" s="14">
+        <f t="shared" ref="D86:J86" si="11">STDEV(D75:D84)</f>
+        <v>0.27752076999348674</v>
+      </c>
+      <c r="E86" s="14">
+        <f t="shared" si="11"/>
+        <v>0.21994948915098153</v>
+      </c>
+      <c r="F86" s="14">
+        <f t="shared" si="11"/>
+        <v>0.16260381299342277</v>
+      </c>
+      <c r="G86" s="14">
+        <f t="shared" si="11"/>
+        <v>0.36866124167195963</v>
+      </c>
+      <c r="H86" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I86" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J86" s="14" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="12"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C89" s="16"/>
+      <c r="D89" s="16"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
+      <c r="I89" s="16"/>
+      <c r="J89" s="16"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="12"/>
+      <c r="B104" s="12"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="12"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="13"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C105" s="16"/>
+      <c r="D105" s="16"/>
+      <c r="E105" s="17"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="I105" s="16"/>
+      <c r="J105" s="16"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" s="12"/>
+      <c r="B120" s="12"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+      <c r="G120" s="12"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="13"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C121" s="16"/>
+      <c r="D121" s="16"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="18"/>
+      <c r="G121" s="18"/>
+      <c r="I121" s="16"/>
+      <c r="J121" s="16"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" s="12"/>
+      <c r="B136" s="12"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="12"/>
+      <c r="E136" s="12"/>
+      <c r="F136" s="12"/>
+      <c r="G136" s="12"/>
+      <c r="H136" s="13"/>
+      <c r="I136" s="13"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C137" s="16"/>
+      <c r="D137" s="16"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="18"/>
+      <c r="G137" s="18"/>
+      <c r="I137" s="16"/>
+      <c r="J137" s="16"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152" s="12"/>
+      <c r="B152" s="12"/>
+      <c r="C152" s="12"/>
+      <c r="D152" s="12"/>
+      <c r="E152" s="12"/>
+      <c r="F152" s="12"/>
+      <c r="G152" s="12"/>
+      <c r="H152" s="13"/>
+      <c r="I152" s="13"/>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C153" s="16"/>
+      <c r="D153" s="16"/>
+      <c r="E153" s="17"/>
+      <c r="F153" s="18"/>
+      <c r="G153" s="18"/>
+      <c r="I153" s="16"/>
+      <c r="J153" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="39">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="I89:J89"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="I105:J105"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="I121:J121"/>
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="F137:G137"/>
+    <mergeCell ref="I137:J137"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="F153:G153"/>
+    <mergeCell ref="I153:J153"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>